<commit_message>
v1.0.10 Add analyses for all three `MCP1`, `MCP1_pg_ml_2015`, and `MCP1_pg_ug_2015`. Add comparison between `MCP1`, `MCP1_pg_ml_2015`, and `MCP1_pg_ug_2015`. Add (and fixed) ordinal regression. Double checked which measurement to use.
</commit_message>
<xml_diff>
--- a/IL6MCP1/BASELINE/20200625.IL6MCP1.AE.BaselineTable.subsetCEA.xlsx
+++ b/IL6MCP1/BASELINE/20200625.IL6MCP1.AE.BaselineTable.subsetCEA.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="590">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="591">
   <si>
     <t xml:space="preserve"/>
   </si>
@@ -41,7 +41,7 @@
     <t xml:space="preserve">    161</t>
   </si>
   <si>
-    <t xml:space="preserve">   1165</t>
+    <t xml:space="preserve">   1167</t>
   </si>
   <si>
     <t xml:space="preserve">    </t>
@@ -56,10 +56,10 @@
     <t xml:space="preserve">   52.2 ( 84) </t>
   </si>
   <si>
-    <t xml:space="preserve">   47.0 ( 547) </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.246</t>
+    <t xml:space="preserve">   46.9 ( 547) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.239</t>
   </si>
   <si>
     <t xml:space="preserve"> 0.0</t>
@@ -74,7 +74,7 @@
     <t xml:space="preserve">   47.8 ( 77) </t>
   </si>
   <si>
-    <t xml:space="preserve">   53.0 ( 618) </t>
+    <t xml:space="preserve">   53.1 ( 620) </t>
   </si>
   <si>
     <t xml:space="preserve">ORyear....freq.</t>
@@ -149,7 +149,7 @@
     <t xml:space="preserve">    8.7 ( 14) </t>
   </si>
   <si>
-    <t xml:space="preserve">   10.0 ( 116) </t>
+    <t xml:space="preserve">    9.9 ( 116) </t>
   </si>
   <si>
     <t xml:space="preserve">X.6</t>
@@ -182,7 +182,7 @@
     <t xml:space="preserve">2009</t>
   </si>
   <si>
-    <t xml:space="preserve">    7.6 (  89) </t>
+    <t xml:space="preserve">    7.7 (  90) </t>
   </si>
   <si>
     <t xml:space="preserve">X.9</t>
@@ -194,7 +194,7 @@
     <t xml:space="preserve">    4.3 (  7) </t>
   </si>
   <si>
-    <t xml:space="preserve">    7.0 (  81) </t>
+    <t xml:space="preserve">    6.9 (  81) </t>
   </si>
   <si>
     <t xml:space="preserve">X.10</t>
@@ -206,7 +206,7 @@
     <t xml:space="preserve">    5.0 (  8) </t>
   </si>
   <si>
-    <t xml:space="preserve">    8.7 ( 101) </t>
+    <t xml:space="preserve">    8.7 ( 102) </t>
   </si>
   <si>
     <t xml:space="preserve">X.11</t>
@@ -215,7 +215,7 @@
     <t xml:space="preserve">2012</t>
   </si>
   <si>
-    <t xml:space="preserve">    7.6 (  88) </t>
+    <t xml:space="preserve">    7.5 (  88) </t>
   </si>
   <si>
     <t xml:space="preserve">X.12</t>
@@ -272,7 +272,7 @@
     <t xml:space="preserve"> 65.901 (9.051)</t>
   </si>
   <si>
-    <t xml:space="preserve"> 68.788 (9.081)</t>
+    <t xml:space="preserve"> 68.785 (9.081)</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;0.001</t>
@@ -287,10 +287,10 @@
     <t xml:space="preserve">   23.0 ( 37) </t>
   </si>
   <si>
-    <t xml:space="preserve">   30.4 ( 354) </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.066</t>
+    <t xml:space="preserve">   30.4 ( 355) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.065</t>
   </si>
   <si>
     <t xml:space="preserve">X.19</t>
@@ -302,7 +302,7 @@
     <t xml:space="preserve">   77.0 (124) </t>
   </si>
   <si>
-    <t xml:space="preserve">   69.6 ( 811) </t>
+    <t xml:space="preserve">   69.6 ( 812) </t>
   </si>
   <si>
     <t xml:space="preserve">TC_finalCU..mean..SD..</t>
@@ -311,13 +311,13 @@
     <t xml:space="preserve">179.199 (45.274)</t>
   </si>
   <si>
-    <t xml:space="preserve">183.983 (48.290)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.331</t>
-  </si>
-  <si>
-    <t xml:space="preserve">32.7</t>
+    <t xml:space="preserve">184.078 (48.333)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.322</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32.8</t>
   </si>
   <si>
     <t xml:space="preserve">LDL_finalCU..mean..SD..</t>
@@ -326,10 +326,10 @@
     <t xml:space="preserve">104.132 (37.590)</t>
   </si>
   <si>
-    <t xml:space="preserve">109.642 (41.227)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.215</t>
+    <t xml:space="preserve">109.761 (41.318)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.206</t>
   </si>
   <si>
     <t xml:space="preserve">39.8</t>
@@ -341,10 +341,10 @@
     <t xml:space="preserve"> 44.749 (14.890)</t>
   </si>
   <si>
-    <t xml:space="preserve"> 45.808 (18.231)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.568</t>
+    <t xml:space="preserve"> 45.803 (18.219)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.570</t>
   </si>
   <si>
     <t xml:space="preserve">36.1</t>
@@ -356,10 +356,10 @@
     <t xml:space="preserve">158.699 (87.584)</t>
   </si>
   <si>
-    <t xml:space="preserve">145.942 (83.223)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.143</t>
+    <t xml:space="preserve">145.901 (83.176)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.141</t>
   </si>
   <si>
     <t xml:space="preserve">35.6</t>
@@ -371,7 +371,7 @@
     <t xml:space="preserve">  4.641 (1.173)</t>
   </si>
   <si>
-    <t xml:space="preserve">  4.765 (1.251)</t>
+    <t xml:space="preserve">  4.768 (1.252)</t>
   </si>
   <si>
     <t xml:space="preserve">LDL_final..mean..SD..</t>
@@ -380,7 +380,7 @@
     <t xml:space="preserve">  2.697 (0.974)</t>
   </si>
   <si>
-    <t xml:space="preserve">  2.840 (1.068)</t>
+    <t xml:space="preserve">  2.843 (1.070)</t>
   </si>
   <si>
     <t xml:space="preserve">HDL_final..mean..SD..</t>
@@ -407,10 +407,10 @@
     <t xml:space="preserve">  6.846 (21.838)</t>
   </si>
   <si>
-    <t xml:space="preserve"> 16.213 (110.899)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.393</t>
+    <t xml:space="preserve"> 16.179 (110.739)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.394</t>
   </si>
   <si>
     <t xml:space="preserve">40.6</t>
@@ -422,10 +422,10 @@
     <t xml:space="preserve">152.838 (24.600)</t>
   </si>
   <si>
-    <t xml:space="preserve">155.742 (26.411)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.225</t>
+    <t xml:space="preserve">155.713 (26.406)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.230</t>
   </si>
   <si>
     <t xml:space="preserve">13.5</t>
@@ -437,10 +437,10 @@
     <t xml:space="preserve"> 80.824 (12.855)</t>
   </si>
   <si>
-    <t xml:space="preserve"> 82.873 (13.549)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.096</t>
+    <t xml:space="preserve"> 82.863 (13.542)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.097</t>
   </si>
   <si>
     <t xml:space="preserve">GFR_MDRD..mean..SD..</t>
@@ -449,10 +449,10 @@
     <t xml:space="preserve"> 70.440 (19.793)</t>
   </si>
   <si>
-    <t xml:space="preserve"> 71.901 (20.142)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.396</t>
+    <t xml:space="preserve"> 71.890 (20.127)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.400</t>
   </si>
   <si>
     <t xml:space="preserve"> 3.5</t>
@@ -464,10 +464,10 @@
     <t xml:space="preserve"> 26.626 (3.572)</t>
   </si>
   <si>
-    <t xml:space="preserve"> 26.350 (3.768)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.389</t>
+    <t xml:space="preserve"> 26.350 (3.765)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.387</t>
   </si>
   <si>
     <t xml:space="preserve"> 4.4</t>
@@ -497,7 +497,7 @@
     <t xml:space="preserve">   50.9 ( 82) </t>
   </si>
   <si>
-    <t xml:space="preserve">   53.4 ( 622) </t>
+    <t xml:space="preserve">   53.4 ( 623) </t>
   </si>
   <si>
     <t xml:space="preserve">X.22</t>
@@ -509,7 +509,7 @@
     <t xml:space="preserve">   29.8 ( 48) </t>
   </si>
   <si>
-    <t xml:space="preserve">   23.9 ( 279) </t>
+    <t xml:space="preserve">   24.0 ( 280) </t>
   </si>
   <si>
     <t xml:space="preserve">X.23</t>
@@ -569,7 +569,7 @@
     <t xml:space="preserve">   32.3 ( 52) </t>
   </si>
   <si>
-    <t xml:space="preserve">   35.5 ( 414) </t>
+    <t xml:space="preserve">   35.6 ( 415) </t>
   </si>
   <si>
     <t xml:space="preserve">X.28</t>
@@ -581,7 +581,7 @@
     <t xml:space="preserve">   49.7 ( 80) </t>
   </si>
   <si>
-    <t xml:space="preserve">   45.6 ( 531) </t>
+    <t xml:space="preserve">   45.6 ( 532) </t>
   </si>
   <si>
     <t xml:space="preserve">X.29</t>
@@ -608,10 +608,10 @@
     <t xml:space="preserve">   29.2 ( 47) </t>
   </si>
   <si>
-    <t xml:space="preserve">   36.0 ( 419) </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.072</t>
+    <t xml:space="preserve">   36.1 ( 421) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.069</t>
   </si>
   <si>
     <t xml:space="preserve"> 4.0</t>
@@ -626,16 +626,13 @@
     <t xml:space="preserve">   56.5 ( 91) </t>
   </si>
   <si>
-    <t xml:space="preserve">   45.7 ( 532) </t>
-  </si>
-  <si>
     <t xml:space="preserve">X.32</t>
   </si>
   <si>
     <t xml:space="preserve">Never smoked</t>
   </si>
   <si>
-    <t xml:space="preserve">   14.2 ( 165) </t>
+    <t xml:space="preserve">   14.1 ( 165) </t>
   </si>
   <si>
     <t xml:space="preserve">X.33</t>
@@ -659,10 +656,10 @@
     <t xml:space="preserve">   33.6 ( 392) </t>
   </si>
   <si>
-    <t xml:space="preserve"> 0.223</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 3.8</t>
+    <t xml:space="preserve"> 0.210</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3.9</t>
   </si>
   <si>
     <t xml:space="preserve">X.34</t>
@@ -674,7 +671,7 @@
     <t xml:space="preserve">   59.6 ( 96) </t>
   </si>
   <si>
-    <t xml:space="preserve">   62.2 ( 725) </t>
+    <t xml:space="preserve">   62.2 ( 726) </t>
   </si>
   <si>
     <t xml:space="preserve">X.35</t>
@@ -683,9 +680,6 @@
     <t xml:space="preserve">    1.9 (  3) </t>
   </si>
   <si>
-    <t xml:space="preserve">    4.1 (  48) </t>
-  </si>
-  <si>
     <t xml:space="preserve">DiabetesStatus....freq.</t>
   </si>
   <si>
@@ -695,10 +689,10 @@
     <t xml:space="preserve">   78.3 (126) </t>
   </si>
   <si>
-    <t xml:space="preserve">   77.3 ( 900) </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.852</t>
+    <t xml:space="preserve">   77.3 ( 902) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.861</t>
   </si>
   <si>
     <t xml:space="preserve">X.36</t>
@@ -728,7 +722,7 @@
     <t xml:space="preserve">   25.5 ( 41) </t>
   </si>
   <si>
-    <t xml:space="preserve">   26.5 ( 309) </t>
+    <t xml:space="preserve">   26.6 ( 310) </t>
   </si>
   <si>
     <t xml:space="preserve">X.38</t>
@@ -740,7 +734,7 @@
     <t xml:space="preserve">   73.9 (119) </t>
   </si>
   <si>
-    <t xml:space="preserve">   71.4 ( 832) </t>
+    <t xml:space="preserve">   71.4 ( 833) </t>
   </si>
   <si>
     <t xml:space="preserve">X.39</t>
@@ -758,7 +752,7 @@
     <t xml:space="preserve">X.40</t>
   </si>
   <si>
-    <t xml:space="preserve">   32.9 ( 383) </t>
+    <t xml:space="preserve">   32.9 ( 384) </t>
   </si>
   <si>
     <t xml:space="preserve">X.41</t>
@@ -767,7 +761,7 @@
     <t xml:space="preserve">   66.5 (107) </t>
   </si>
   <si>
-    <t xml:space="preserve">   64.5 ( 752) </t>
+    <t xml:space="preserve">   64.5 ( 753) </t>
   </si>
   <si>
     <t xml:space="preserve">X.42</t>
@@ -785,16 +779,13 @@
     <t xml:space="preserve">   11.2 ( 18) </t>
   </si>
   <si>
-    <t xml:space="preserve">   14.1 ( 164) </t>
-  </si>
-  <si>
     <t xml:space="preserve">X.44</t>
   </si>
   <si>
     <t xml:space="preserve">   88.8 (143) </t>
   </si>
   <si>
-    <t xml:space="preserve">   85.9 (1001) </t>
+    <t xml:space="preserve">   85.9 (1002) </t>
   </si>
   <si>
     <t xml:space="preserve">Hypertension.drugs....freq.</t>
@@ -809,13 +800,16 @@
     <t xml:space="preserve">   15.5 ( 25) </t>
   </si>
   <si>
+    <t xml:space="preserve">   22.8 ( 266) </t>
+  </si>
+  <si>
     <t xml:space="preserve">X.46</t>
   </si>
   <si>
     <t xml:space="preserve">   83.9 (135) </t>
   </si>
   <si>
-    <t xml:space="preserve">   77.1 ( 898) </t>
+    <t xml:space="preserve">   77.0 ( 899) </t>
   </si>
   <si>
     <t xml:space="preserve">X.47</t>
@@ -833,7 +827,7 @@
     <t xml:space="preserve">   89.4 (144) </t>
   </si>
   <si>
-    <t xml:space="preserve">   88.0 (1025) </t>
+    <t xml:space="preserve">   88.0 (1027) </t>
   </si>
   <si>
     <t xml:space="preserve">X.49</t>
@@ -866,7 +860,7 @@
     <t xml:space="preserve">   92.5 (149) </t>
   </si>
   <si>
-    <t xml:space="preserve">   88.8 (1035) </t>
+    <t xml:space="preserve">   88.9 (1037) </t>
   </si>
   <si>
     <t xml:space="preserve">X.53</t>
@@ -884,7 +878,7 @@
     <t xml:space="preserve">   17.4 ( 28) </t>
   </si>
   <si>
-    <t xml:space="preserve">   23.2 ( 270) </t>
+    <t xml:space="preserve">   23.1 ( 270) </t>
   </si>
   <si>
     <t xml:space="preserve">X.55</t>
@@ -893,7 +887,7 @@
     <t xml:space="preserve">   82.0 (132) </t>
   </si>
   <si>
-    <t xml:space="preserve">   76.7 ( 893) </t>
+    <t xml:space="preserve">   76.7 ( 895) </t>
   </si>
   <si>
     <t xml:space="preserve">X.56</t>
@@ -914,7 +908,7 @@
     <t xml:space="preserve">   80.1 (129) </t>
   </si>
   <si>
-    <t xml:space="preserve">   75.5 ( 880) </t>
+    <t xml:space="preserve">   75.5 ( 881) </t>
   </si>
   <si>
     <t xml:space="preserve">X.58</t>
@@ -923,7 +917,7 @@
     <t xml:space="preserve">Stroke diagnosed</t>
   </si>
   <si>
-    <t xml:space="preserve">   19.1 ( 222) </t>
+    <t xml:space="preserve">   19.1 ( 223) </t>
   </si>
   <si>
     <t xml:space="preserve">X.59</t>
@@ -950,7 +944,7 @@
     <t xml:space="preserve">TIA</t>
   </si>
   <si>
-    <t xml:space="preserve">   46.6 ( 543) </t>
+    <t xml:space="preserve">   46.5 ( 543) </t>
   </si>
   <si>
     <t xml:space="preserve">X.62</t>
@@ -959,7 +953,7 @@
     <t xml:space="preserve">minor stroke</t>
   </si>
   <si>
-    <t xml:space="preserve">   17.2 ( 200) </t>
+    <t xml:space="preserve">   17.1 ( 200) </t>
   </si>
   <si>
     <t xml:space="preserve">X.63</t>
@@ -968,7 +962,7 @@
     <t xml:space="preserve">Major stroke</t>
   </si>
   <si>
-    <t xml:space="preserve">   11.6 ( 135) </t>
+    <t xml:space="preserve">   11.7 ( 136) </t>
   </si>
   <si>
     <t xml:space="preserve">X.64</t>
@@ -977,7 +971,7 @@
     <t xml:space="preserve">Amaurosis fugax</t>
   </si>
   <si>
-    <t xml:space="preserve">   16.9 ( 197) </t>
+    <t xml:space="preserve">   17.0 ( 198) </t>
   </si>
   <si>
     <t xml:space="preserve">X.65</t>
@@ -1076,7 +1070,7 @@
     <t xml:space="preserve">Ocular</t>
   </si>
   <si>
-    <t xml:space="preserve">   17.0 ( 198) </t>
+    <t xml:space="preserve">   17.1 ( 199) </t>
   </si>
   <si>
     <t xml:space="preserve">X.78</t>
@@ -1100,13 +1094,13 @@
     <t xml:space="preserve">Stroke</t>
   </si>
   <si>
-    <t xml:space="preserve">   28.8 ( 335) </t>
+    <t xml:space="preserve">   28.8 ( 336) </t>
   </si>
   <si>
     <t xml:space="preserve">X.81</t>
   </si>
   <si>
-    <t xml:space="preserve">   46.8 ( 545) </t>
+    <t xml:space="preserve">   46.7 ( 545) </t>
   </si>
   <si>
     <t xml:space="preserve">AsymptSympt....freq.</t>
@@ -1118,7 +1112,7 @@
     <t xml:space="preserve">Ocular and others</t>
   </si>
   <si>
-    <t xml:space="preserve">   24.5 ( 285) </t>
+    <t xml:space="preserve">   24.5 ( 286) </t>
   </si>
   <si>
     <t xml:space="preserve">X.83</t>
@@ -1130,7 +1124,7 @@
     <t xml:space="preserve">X.84</t>
   </si>
   <si>
-    <t xml:space="preserve">  100.0 (1165) </t>
+    <t xml:space="preserve">  100.0 (1167) </t>
   </si>
   <si>
     <t xml:space="preserve">restenos....freq.</t>
@@ -1148,7 +1142,7 @@
     <t xml:space="preserve">   93.2 (150) </t>
   </si>
   <si>
-    <t xml:space="preserve">   95.0 (1107) </t>
+    <t xml:space="preserve">   95.0 (1109) </t>
   </si>
   <si>
     <t xml:space="preserve">X.86</t>
@@ -1190,7 +1184,7 @@
     <t xml:space="preserve">50-70%</t>
   </si>
   <si>
-    <t xml:space="preserve">    6.2 (  72) </t>
+    <t xml:space="preserve">    6.3 (  73) </t>
   </si>
   <si>
     <t xml:space="preserve">X.91</t>
@@ -1211,7 +1205,7 @@
     <t xml:space="preserve">   42.9 ( 69) </t>
   </si>
   <si>
-    <t xml:space="preserve">   43.3 ( 504) </t>
+    <t xml:space="preserve">   43.3 ( 505) </t>
   </si>
   <si>
     <t xml:space="preserve">X.93</t>
@@ -1259,10 +1253,10 @@
     <t xml:space="preserve">   37.3 ( 60) </t>
   </si>
   <si>
-    <t xml:space="preserve">   36.7 ( 428) </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.965</t>
+    <t xml:space="preserve">   36.8 ( 429) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.970</t>
   </si>
   <si>
     <t xml:space="preserve">X.99</t>
@@ -1271,7 +1265,7 @@
     <t xml:space="preserve">   62.7 (101) </t>
   </si>
   <si>
-    <t xml:space="preserve">   63.3 ( 737) </t>
+    <t xml:space="preserve">   63.2 ( 738) </t>
   </si>
   <si>
     <t xml:space="preserve">CAD_history....freq.</t>
@@ -1286,7 +1280,7 @@
     <t xml:space="preserve">   59.0 ( 95) </t>
   </si>
   <si>
-    <t xml:space="preserve">   69.1 ( 805) </t>
+    <t xml:space="preserve">   69.2 ( 807) </t>
   </si>
   <si>
     <t xml:space="preserve">X.101</t>
@@ -1298,7 +1292,7 @@
     <t xml:space="preserve">   41.0 ( 66) </t>
   </si>
   <si>
-    <t xml:space="preserve">   30.9 ( 360) </t>
+    <t xml:space="preserve">   30.8 ( 360) </t>
   </si>
   <si>
     <t xml:space="preserve">PAOD....freq.</t>
@@ -1310,7 +1304,7 @@
     <t xml:space="preserve">X.102</t>
   </si>
   <si>
-    <t xml:space="preserve">   79.8 ( 930) </t>
+    <t xml:space="preserve">   79.9 ( 932) </t>
   </si>
   <si>
     <t xml:space="preserve">X.103</t>
@@ -1319,7 +1313,7 @@
     <t xml:space="preserve">   26.1 ( 42) </t>
   </si>
   <si>
-    <t xml:space="preserve">   20.2 ( 235) </t>
+    <t xml:space="preserve">   20.1 ( 235) </t>
   </si>
   <si>
     <t xml:space="preserve">Peripheral.interv....freq.</t>
@@ -1328,7 +1322,7 @@
     <t xml:space="preserve">   72.7 (117) </t>
   </si>
   <si>
-    <t xml:space="preserve">   83.0 ( 967) </t>
+    <t xml:space="preserve">   83.0 ( 969) </t>
   </si>
   <si>
     <t xml:space="preserve"> 0.004</t>
@@ -1364,7 +1358,7 @@
     <t xml:space="preserve">   68.3 (110) </t>
   </si>
   <si>
-    <t xml:space="preserve">   73.8 ( 860) </t>
+    <t xml:space="preserve">   73.9 ( 862) </t>
   </si>
   <si>
     <t xml:space="preserve">X.107</t>
@@ -1388,10 +1382,10 @@
     <t xml:space="preserve">  2.579 (0.961)</t>
   </si>
   <si>
-    <t xml:space="preserve">  2.611 (1.130)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.735</t>
+    <t xml:space="preserve">  2.612 (1.129)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.729</t>
   </si>
   <si>
     <t xml:space="preserve"> 1.0</t>
@@ -1403,10 +1397,10 @@
     <t xml:space="preserve">  0.802 (1.072)</t>
   </si>
   <si>
-    <t xml:space="preserve">  0.822 (1.275)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.856</t>
+    <t xml:space="preserve">  0.821 (1.275)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.862</t>
   </si>
   <si>
     <t xml:space="preserve"> 2.2</t>
@@ -1418,7 +1412,7 @@
     <t xml:space="preserve">  2.445 (2.594)</t>
   </si>
   <si>
-    <t xml:space="preserve">  1.923 (2.234)</t>
+    <t xml:space="preserve">  1.924 (2.233)</t>
   </si>
   <si>
     <t xml:space="preserve"> 0.007</t>
@@ -1436,10 +1430,10 @@
     <t xml:space="preserve">   50.3 ( 81) </t>
   </si>
   <si>
-    <t xml:space="preserve">   45.8 ( 533) </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.309</t>
+    <t xml:space="preserve">   45.8 ( 534) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.311</t>
   </si>
   <si>
     <t xml:space="preserve"> 1.8</t>
@@ -1454,7 +1448,7 @@
     <t xml:space="preserve">   49.1 ( 79) </t>
   </si>
   <si>
-    <t xml:space="preserve">   52.3 ( 609) </t>
+    <t xml:space="preserve">   52.3 ( 610) </t>
   </si>
   <si>
     <t xml:space="preserve">X.110</t>
@@ -1469,7 +1463,7 @@
     <t xml:space="preserve">   32.5 ( 379) </t>
   </si>
   <si>
-    <t xml:space="preserve"> 0.017</t>
+    <t xml:space="preserve"> 0.018</t>
   </si>
   <si>
     <t xml:space="preserve"> 1.7</t>
@@ -1478,7 +1472,7 @@
     <t xml:space="preserve">X.111</t>
   </si>
   <si>
-    <t xml:space="preserve">   65.8 ( 766) </t>
+    <t xml:space="preserve">   65.8 ( 768) </t>
   </si>
   <si>
     <t xml:space="preserve">X.112</t>
@@ -1511,9 +1505,6 @@
     <t xml:space="preserve">173.244 (168.601)</t>
   </si>
   <si>
-    <t xml:space="preserve"> 0.097</t>
-  </si>
-  <si>
     <t xml:space="preserve">83.7</t>
   </si>
   <si>
@@ -1523,10 +1514,10 @@
     <t xml:space="preserve">   39.1 ( 63) </t>
   </si>
   <si>
-    <t xml:space="preserve">   36.3 ( 423) </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.512</t>
+    <t xml:space="preserve">   36.4 ( 425) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.521</t>
   </si>
   <si>
     <t xml:space="preserve"> 1.5</t>
@@ -1538,7 +1529,7 @@
     <t xml:space="preserve">   60.2 ( 97) </t>
   </si>
   <si>
-    <t xml:space="preserve">   62.1 ( 723) </t>
+    <t xml:space="preserve">   62.0 ( 723) </t>
   </si>
   <si>
     <t xml:space="preserve">X.114</t>
@@ -1550,10 +1541,10 @@
     <t xml:space="preserve">  8.837 (6.727)</t>
   </si>
   <si>
-    <t xml:space="preserve">  8.439 (6.394)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.480</t>
+    <t xml:space="preserve">  8.438 (6.388)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.478</t>
   </si>
   <si>
     <t xml:space="preserve"> 8.0</t>
@@ -1562,7 +1553,7 @@
     <t xml:space="preserve">Calc.bin....freq.</t>
   </si>
   <si>
-    <t xml:space="preserve">   51.2 ( 596) </t>
+    <t xml:space="preserve">   51.2 ( 597) </t>
   </si>
   <si>
     <t xml:space="preserve"> 0.003</t>
@@ -1577,7 +1568,7 @@
     <t xml:space="preserve">   60.9 ( 98) </t>
   </si>
   <si>
-    <t xml:space="preserve">   47.3 ( 551) </t>
+    <t xml:space="preserve">   47.3 ( 552) </t>
   </si>
   <si>
     <t xml:space="preserve">X.116</t>
@@ -1595,7 +1586,7 @@
     <t xml:space="preserve">   20.7 ( 241) </t>
   </si>
   <si>
-    <t xml:space="preserve"> 0.523</t>
+    <t xml:space="preserve"> 0.528</t>
   </si>
   <si>
     <t xml:space="preserve">X.117</t>
@@ -1604,7 +1595,7 @@
     <t xml:space="preserve">   80.7 (130) </t>
   </si>
   <si>
-    <t xml:space="preserve">   77.8 ( 906) </t>
+    <t xml:space="preserve">   77.8 ( 908) </t>
   </si>
   <si>
     <t xml:space="preserve">X.118</t>
@@ -1619,10 +1610,10 @@
     <t xml:space="preserve">   35.4 ( 57) </t>
   </si>
   <si>
-    <t xml:space="preserve">   25.8 ( 300) </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.014</t>
+    <t xml:space="preserve">   25.7 ( 300) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.013</t>
   </si>
   <si>
     <t xml:space="preserve"> 1.3</t>
@@ -1637,7 +1628,7 @@
     <t xml:space="preserve">   64.6 (104) </t>
   </si>
   <si>
-    <t xml:space="preserve">   72.8 ( 848) </t>
+    <t xml:space="preserve">   72.8 ( 850) </t>
   </si>
   <si>
     <t xml:space="preserve">X.120</t>
@@ -1652,10 +1643,10 @@
     <t xml:space="preserve">&lt;40%</t>
   </si>
   <si>
-    <t xml:space="preserve">   70.5 ( 821) </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.060</t>
+    <t xml:space="preserve">   70.5 ( 823) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.061</t>
   </si>
   <si>
     <t xml:space="preserve">X.121</t>
@@ -1664,7 +1655,7 @@
     <t xml:space="preserve">&gt;40%</t>
   </si>
   <si>
-    <t xml:space="preserve">   28.1 ( 327) </t>
+    <t xml:space="preserve">   28.0 ( 327) </t>
   </si>
   <si>
     <t xml:space="preserve">X.122</t>
@@ -1703,7 +1694,7 @@
     <t xml:space="preserve">   45.3 ( 73) </t>
   </si>
   <si>
-    <t xml:space="preserve">   33.6 ( 391) </t>
+    <t xml:space="preserve">   33.5 ( 391) </t>
   </si>
   <si>
     <t xml:space="preserve">X.125</t>
@@ -1721,7 +1712,7 @@
     <t xml:space="preserve"> 0.616</t>
   </si>
   <si>
-    <t xml:space="preserve">61.0</t>
+    <t xml:space="preserve">61.1</t>
   </si>
   <si>
     <t xml:space="preserve">IL6_pg_ug_2015..mean..SD..</t>
@@ -1748,7 +1739,7 @@
     <t xml:space="preserve">  0.209 (0.250)</t>
   </si>
   <si>
-    <t xml:space="preserve"> 0.313</t>
+    <t xml:space="preserve"> 0.306</t>
   </si>
   <si>
     <t xml:space="preserve">13.1</t>
@@ -1766,7 +1757,7 @@
     <t xml:space="preserve"> 0.063</t>
   </si>
   <si>
-    <t xml:space="preserve">57.4</t>
+    <t xml:space="preserve">57.5</t>
   </si>
   <si>
     <t xml:space="preserve">MCP1_pg_ug_2015..mean..SD..</t>
@@ -1775,13 +1766,25 @@
     <t xml:space="preserve">  0.495 (0.818)</t>
   </si>
   <si>
-    <t xml:space="preserve">  0.626 (0.915)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.117</t>
+    <t xml:space="preserve">  0.627 (0.914)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.116</t>
   </si>
   <si>
     <t xml:space="preserve"> 9.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCP1_pg_ml_2015..mean..SD..</t>
+  </si>
+  <si>
+    <t xml:space="preserve">405.182 (563.654)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">624.885 (885.359)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.006</t>
   </si>
 </sst>
 </file>
@@ -3339,7 +3342,7 @@
         <v>203</v>
       </c>
       <c r="D54" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="E54" t="s">
         <v>0</v>
@@ -3353,16 +3356,16 @@
     </row>
     <row r="55">
       <c r="A55" t="s">
+        <v>204</v>
+      </c>
+      <c r="B55" t="s">
         <v>205</v>
-      </c>
-      <c r="B55" t="s">
-        <v>206</v>
       </c>
       <c r="C55" t="s">
         <v>32</v>
       </c>
       <c r="D55" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E55" t="s">
         <v>0</v>
@@ -3376,14 +3379,14 @@
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B56"/>
       <c r="C56" t="s">
+        <v>208</v>
+      </c>
+      <c r="D56" t="s">
         <v>209</v>
-      </c>
-      <c r="D56" t="s">
-        <v>210</v>
       </c>
       <c r="E56" t="s">
         <v>0</v>
@@ -3397,39 +3400,39 @@
     </row>
     <row r="57">
       <c r="A57" t="s">
+        <v>210</v>
+      </c>
+      <c r="B57" t="s">
         <v>211</v>
       </c>
-      <c r="B57" t="s">
+      <c r="C57" t="s">
         <v>212</v>
       </c>
-      <c r="C57" t="s">
+      <c r="D57" t="s">
         <v>213</v>
       </c>
-      <c r="D57" t="s">
+      <c r="E57" t="s">
         <v>214</v>
       </c>
-      <c r="E57" t="s">
+      <c r="F57" t="s">
+        <v>0</v>
+      </c>
+      <c r="G57" t="s">
         <v>215</v>
-      </c>
-      <c r="F57" t="s">
-        <v>0</v>
-      </c>
-      <c r="G57" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
+        <v>216</v>
+      </c>
+      <c r="B58" t="s">
         <v>217</v>
       </c>
-      <c r="B58" t="s">
+      <c r="C58" t="s">
         <v>218</v>
       </c>
-      <c r="C58" t="s">
+      <c r="D58" t="s">
         <v>219</v>
-      </c>
-      <c r="D58" t="s">
-        <v>220</v>
       </c>
       <c r="E58" t="s">
         <v>0</v>
@@ -3443,14 +3446,14 @@
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B59"/>
       <c r="C59" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D59" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="E59" t="s">
         <v>0</v>
@@ -3464,19 +3467,19 @@
     </row>
     <row r="60">
       <c r="A60" t="s">
+        <v>222</v>
+      </c>
+      <c r="B60" t="s">
+        <v>223</v>
+      </c>
+      <c r="C60" t="s">
         <v>224</v>
       </c>
-      <c r="B60" t="s">
+      <c r="D60" t="s">
         <v>225</v>
       </c>
-      <c r="C60" t="s">
+      <c r="E60" t="s">
         <v>226</v>
-      </c>
-      <c r="D60" t="s">
-        <v>227</v>
-      </c>
-      <c r="E60" t="s">
-        <v>228</v>
       </c>
       <c r="F60" t="s">
         <v>0</v>
@@ -3487,16 +3490,16 @@
     </row>
     <row r="61">
       <c r="A61" t="s">
+        <v>227</v>
+      </c>
+      <c r="B61" t="s">
+        <v>228</v>
+      </c>
+      <c r="C61" t="s">
         <v>229</v>
       </c>
-      <c r="B61" t="s">
+      <c r="D61" t="s">
         <v>230</v>
-      </c>
-      <c r="C61" t="s">
-        <v>231</v>
-      </c>
-      <c r="D61" t="s">
-        <v>232</v>
       </c>
       <c r="E61" t="s">
         <v>0</v>
@@ -3510,7 +3513,7 @@
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B62" t="s">
         <v>22</v>
@@ -3528,21 +3531,21 @@
         <v>0</v>
       </c>
       <c r="G62" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
+        <v>233</v>
+      </c>
+      <c r="B63" t="s">
+        <v>234</v>
+      </c>
+      <c r="C63" t="s">
         <v>235</v>
       </c>
-      <c r="B63" t="s">
+      <c r="D63" t="s">
         <v>236</v>
-      </c>
-      <c r="C63" t="s">
-        <v>237</v>
-      </c>
-      <c r="D63" t="s">
-        <v>238</v>
       </c>
       <c r="E63" t="s">
         <v>0</v>
@@ -3556,16 +3559,16 @@
     </row>
     <row r="64">
       <c r="A64" t="s">
+        <v>237</v>
+      </c>
+      <c r="B64" t="s">
+        <v>238</v>
+      </c>
+      <c r="C64" t="s">
         <v>239</v>
       </c>
-      <c r="B64" t="s">
+      <c r="D64" t="s">
         <v>240</v>
-      </c>
-      <c r="C64" t="s">
-        <v>241</v>
-      </c>
-      <c r="D64" t="s">
-        <v>242</v>
       </c>
       <c r="E64" t="s">
         <v>0</v>
@@ -3579,14 +3582,14 @@
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B65"/>
       <c r="C65" t="s">
         <v>171</v>
       </c>
       <c r="D65" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E65" t="s">
         <v>0</v>
@@ -3600,7 +3603,7 @@
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B66" t="s">
         <v>22</v>
@@ -3618,21 +3621,21 @@
         <v>0</v>
       </c>
       <c r="G66" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B67" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C67" t="s">
         <v>184</v>
       </c>
       <c r="D67" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E67" t="s">
         <v>0</v>
@@ -3646,16 +3649,16 @@
     </row>
     <row r="68">
       <c r="A68" t="s">
+        <v>247</v>
+      </c>
+      <c r="B68" t="s">
+        <v>238</v>
+      </c>
+      <c r="C68" t="s">
+        <v>248</v>
+      </c>
+      <c r="D68" t="s">
         <v>249</v>
-      </c>
-      <c r="B68" t="s">
-        <v>240</v>
-      </c>
-      <c r="C68" t="s">
-        <v>250</v>
-      </c>
-      <c r="D68" t="s">
-        <v>251</v>
       </c>
       <c r="E68" t="s">
         <v>0</v>
@@ -3669,14 +3672,14 @@
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B69"/>
       <c r="C69" t="s">
         <v>180</v>
       </c>
       <c r="D69" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E69" t="s">
         <v>0</v>
@@ -3690,7 +3693,7 @@
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B70" t="s">
         <v>22</v>
@@ -3713,16 +3716,16 @@
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B71" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C71" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D71" t="s">
-        <v>257</v>
+        <v>206</v>
       </c>
       <c r="E71" t="s">
         <v>0</v>
@@ -3736,16 +3739,16 @@
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B72" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C72" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D72" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="E72" t="s">
         <v>0</v>
@@ -3759,7 +3762,7 @@
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B73" t="s">
         <v>22</v>
@@ -3777,21 +3780,21 @@
         <v>0</v>
       </c>
       <c r="G73" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B74" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C74" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D74" t="s">
-        <v>232</v>
+        <v>262</v>
       </c>
       <c r="E74" t="s">
         <v>0</v>
@@ -3805,16 +3808,16 @@
     </row>
     <row r="75">
       <c r="A75" t="s">
+        <v>263</v>
+      </c>
+      <c r="B75" t="s">
+        <v>238</v>
+      </c>
+      <c r="C75" t="s">
+        <v>264</v>
+      </c>
+      <c r="D75" t="s">
         <v>265</v>
-      </c>
-      <c r="B75" t="s">
-        <v>240</v>
-      </c>
-      <c r="C75" t="s">
-        <v>266</v>
-      </c>
-      <c r="D75" t="s">
-        <v>267</v>
       </c>
       <c r="E75" t="s">
         <v>0</v>
@@ -3828,14 +3831,14 @@
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B76"/>
       <c r="C76" t="s">
         <v>171</v>
       </c>
       <c r="D76" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E76" t="s">
         <v>0</v>
@@ -3849,7 +3852,7 @@
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B77" t="s">
         <v>22</v>
@@ -3867,21 +3870,21 @@
         <v>0</v>
       </c>
       <c r="G77" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
+        <v>269</v>
+      </c>
+      <c r="B78" t="s">
+        <v>234</v>
+      </c>
+      <c r="C78" t="s">
+        <v>270</v>
+      </c>
+      <c r="D78" t="s">
         <v>271</v>
-      </c>
-      <c r="B78" t="s">
-        <v>236</v>
-      </c>
-      <c r="C78" t="s">
-        <v>272</v>
-      </c>
-      <c r="D78" t="s">
-        <v>273</v>
       </c>
       <c r="E78" t="s">
         <v>0</v>
@@ -3895,16 +3898,16 @@
     </row>
     <row r="79">
       <c r="A79" t="s">
+        <v>272</v>
+      </c>
+      <c r="B79" t="s">
+        <v>238</v>
+      </c>
+      <c r="C79" t="s">
+        <v>273</v>
+      </c>
+      <c r="D79" t="s">
         <v>274</v>
-      </c>
-      <c r="B79" t="s">
-        <v>240</v>
-      </c>
-      <c r="C79" t="s">
-        <v>275</v>
-      </c>
-      <c r="D79" t="s">
-        <v>276</v>
       </c>
       <c r="E79" t="s">
         <v>0</v>
@@ -3918,14 +3921,14 @@
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B80"/>
       <c r="C80" t="s">
         <v>171</v>
       </c>
       <c r="D80" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E80" t="s">
         <v>0</v>
@@ -3939,7 +3942,7 @@
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B81" t="s">
         <v>22</v>
@@ -3957,21 +3960,21 @@
         <v>0</v>
       </c>
       <c r="G81" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B82" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C82" t="s">
         <v>52</v>
       </c>
       <c r="D82" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E82" t="s">
         <v>0</v>
@@ -3985,16 +3988,16 @@
     </row>
     <row r="83">
       <c r="A83" t="s">
+        <v>280</v>
+      </c>
+      <c r="B83" t="s">
+        <v>238</v>
+      </c>
+      <c r="C83" t="s">
+        <v>281</v>
+      </c>
+      <c r="D83" t="s">
         <v>282</v>
-      </c>
-      <c r="B83" t="s">
-        <v>240</v>
-      </c>
-      <c r="C83" t="s">
-        <v>283</v>
-      </c>
-      <c r="D83" t="s">
-        <v>284</v>
       </c>
       <c r="E83" t="s">
         <v>0</v>
@@ -4008,14 +4011,14 @@
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B84"/>
       <c r="C84" t="s">
         <v>180</v>
       </c>
       <c r="D84" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E84" t="s">
         <v>0</v>
@@ -4029,7 +4032,7 @@
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B85" t="s">
         <v>22</v>
@@ -4047,21 +4050,21 @@
         <v>0</v>
       </c>
       <c r="G85" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
+        <v>286</v>
+      </c>
+      <c r="B86" t="s">
+        <v>234</v>
+      </c>
+      <c r="C86" t="s">
+        <v>287</v>
+      </c>
+      <c r="D86" t="s">
         <v>288</v>
-      </c>
-      <c r="B86" t="s">
-        <v>236</v>
-      </c>
-      <c r="C86" t="s">
-        <v>289</v>
-      </c>
-      <c r="D86" t="s">
-        <v>290</v>
       </c>
       <c r="E86" t="s">
         <v>0</v>
@@ -4075,16 +4078,16 @@
     </row>
     <row r="87">
       <c r="A87" t="s">
+        <v>289</v>
+      </c>
+      <c r="B87" t="s">
+        <v>238</v>
+      </c>
+      <c r="C87" t="s">
+        <v>290</v>
+      </c>
+      <c r="D87" t="s">
         <v>291</v>
-      </c>
-      <c r="B87" t="s">
-        <v>240</v>
-      </c>
-      <c r="C87" t="s">
-        <v>292</v>
-      </c>
-      <c r="D87" t="s">
-        <v>293</v>
       </c>
       <c r="E87" t="s">
         <v>0</v>
@@ -4098,14 +4101,14 @@
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B88"/>
       <c r="C88" t="s">
         <v>171</v>
       </c>
       <c r="D88" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E88" t="s">
         <v>0</v>
@@ -4119,7 +4122,7 @@
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B89" t="s">
         <v>6</v>
@@ -4137,21 +4140,21 @@
         <v>0</v>
       </c>
       <c r="G89" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="s">
+        <v>295</v>
+      </c>
+      <c r="B90" t="s">
+        <v>296</v>
+      </c>
+      <c r="C90" t="s">
         <v>297</v>
       </c>
-      <c r="B90" t="s">
+      <c r="D90" t="s">
         <v>298</v>
-      </c>
-      <c r="C90" t="s">
-        <v>299</v>
-      </c>
-      <c r="D90" t="s">
-        <v>300</v>
       </c>
       <c r="E90" t="s">
         <v>0</v>
@@ -4165,16 +4168,16 @@
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B91" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C91" t="s">
         <v>40</v>
       </c>
       <c r="D91" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E91" t="s">
         <v>0</v>
@@ -4188,14 +4191,14 @@
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B92"/>
       <c r="C92" t="s">
         <v>52</v>
       </c>
       <c r="D92" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="E92" t="s">
         <v>0</v>
@@ -4209,10 +4212,10 @@
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B93" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C93" t="s">
         <v>23</v>
@@ -4232,13 +4235,13 @@
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B94" t="s">
         <v>2</v>
       </c>
       <c r="C94" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D94" t="s">
         <v>24</v>
@@ -4255,16 +4258,16 @@
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B95" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C95" t="s">
         <v>23</v>
       </c>
       <c r="D95" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E95" t="s">
         <v>0</v>
@@ -4278,16 +4281,16 @@
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B96" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C96" t="s">
         <v>23</v>
       </c>
       <c r="D96" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E96" t="s">
         <v>0</v>
@@ -4301,16 +4304,16 @@
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B97" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C97" t="s">
         <v>23</v>
       </c>
       <c r="D97" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="E97" t="s">
         <v>0</v>
@@ -4324,16 +4327,16 @@
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B98" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C98" t="s">
         <v>23</v>
       </c>
       <c r="D98" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E98" t="s">
         <v>0</v>
@@ -4347,16 +4350,16 @@
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B99" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C99" t="s">
         <v>23</v>
       </c>
       <c r="D99" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="E99" t="s">
         <v>0</v>
@@ -4370,16 +4373,16 @@
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B100" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C100" t="s">
         <v>23</v>
       </c>
       <c r="D100" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E100" t="s">
         <v>0</v>
@@ -4393,16 +4396,16 @@
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B101" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C101" t="s">
         <v>23</v>
       </c>
       <c r="D101" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="E101" t="s">
         <v>0</v>
@@ -4416,16 +4419,16 @@
     </row>
     <row r="102">
       <c r="A102" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B102" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C102" t="s">
         <v>23</v>
       </c>
       <c r="D102" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="E102" t="s">
         <v>0</v>
@@ -4439,16 +4442,16 @@
     </row>
     <row r="103">
       <c r="A103" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B103" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C103" t="s">
         <v>23</v>
       </c>
       <c r="D103" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="E103" t="s">
         <v>0</v>
@@ -4462,16 +4465,16 @@
     </row>
     <row r="104">
       <c r="A104" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B104" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C104" t="s">
         <v>23</v>
       </c>
       <c r="D104" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E104" t="s">
         <v>0</v>
@@ -4485,10 +4488,10 @@
     </row>
     <row r="105">
       <c r="A105" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B105" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C105" t="s">
         <v>23</v>
@@ -4508,10 +4511,10 @@
     </row>
     <row r="106">
       <c r="A106" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B106" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C106" t="s">
         <v>23</v>
@@ -4531,10 +4534,10 @@
     </row>
     <row r="107">
       <c r="A107" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B107" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C107" t="s">
         <v>23</v>
@@ -4554,10 +4557,10 @@
     </row>
     <row r="108">
       <c r="A108" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B108" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C108" t="s">
         <v>23</v>
@@ -4577,10 +4580,10 @@
     </row>
     <row r="109">
       <c r="A109" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B109" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C109" t="s">
         <v>23</v>
@@ -4600,10 +4603,10 @@
     </row>
     <row r="110">
       <c r="A110" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B110" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C110" t="s">
         <v>23</v>
@@ -4623,13 +4626,13 @@
     </row>
     <row r="111">
       <c r="A111" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B111" t="s">
         <v>2</v>
       </c>
       <c r="C111" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D111" t="s">
         <v>24</v>
@@ -4646,16 +4649,16 @@
     </row>
     <row r="112">
       <c r="A112" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B112" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C112" t="s">
         <v>23</v>
       </c>
       <c r="D112" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="E112" t="s">
         <v>0</v>
@@ -4669,16 +4672,16 @@
     </row>
     <row r="113">
       <c r="A113" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B113" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C113" t="s">
         <v>23</v>
       </c>
       <c r="D113" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E113" t="s">
         <v>0</v>
@@ -4692,16 +4695,16 @@
     </row>
     <row r="114">
       <c r="A114" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B114" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C114" t="s">
         <v>23</v>
       </c>
       <c r="D114" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="E114" t="s">
         <v>0</v>
@@ -4715,16 +4718,16 @@
     </row>
     <row r="115">
       <c r="A115" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B115" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C115" t="s">
         <v>23</v>
       </c>
       <c r="D115" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="E115" t="s">
         <v>0</v>
@@ -4738,16 +4741,16 @@
     </row>
     <row r="116">
       <c r="A116" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B116" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C116" t="s">
         <v>23</v>
       </c>
       <c r="D116" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="E116" t="s">
         <v>0</v>
@@ -4761,13 +4764,13 @@
     </row>
     <row r="117">
       <c r="A117" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B117" t="s">
         <v>2</v>
       </c>
       <c r="C117" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D117" t="s">
         <v>24</v>
@@ -4784,16 +4787,16 @@
     </row>
     <row r="118">
       <c r="A118" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B118" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C118" t="s">
         <v>23</v>
       </c>
       <c r="D118" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="E118" t="s">
         <v>0</v>
@@ -4807,7 +4810,7 @@
     </row>
     <row r="119">
       <c r="A119" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B119" t="s">
         <v>3</v>
@@ -4816,7 +4819,7 @@
         <v>23</v>
       </c>
       <c r="D119" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E119" t="s">
         <v>0</v>
@@ -4830,13 +4833,13 @@
     </row>
     <row r="120">
       <c r="A120" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B120" t="s">
         <v>2</v>
       </c>
       <c r="C120" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D120" t="s">
         <v>24</v>
@@ -4853,7 +4856,7 @@
     </row>
     <row r="121">
       <c r="A121" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B121" t="s">
         <v>3</v>
@@ -4862,7 +4865,7 @@
         <v>23</v>
       </c>
       <c r="D121" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="E121" t="s">
         <v>0</v>
@@ -4876,10 +4879,10 @@
     </row>
     <row r="122">
       <c r="A122" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B122" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C122" t="s">
         <v>23</v>
@@ -4894,21 +4897,21 @@
         <v>0</v>
       </c>
       <c r="G122" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="s">
+        <v>373</v>
+      </c>
+      <c r="B123" t="s">
+        <v>374</v>
+      </c>
+      <c r="C123" t="s">
         <v>375</v>
       </c>
-      <c r="B123" t="s">
+      <c r="D123" t="s">
         <v>376</v>
-      </c>
-      <c r="C123" t="s">
-        <v>377</v>
-      </c>
-      <c r="D123" t="s">
-        <v>378</v>
       </c>
       <c r="E123" t="s">
         <v>0</v>
@@ -4922,16 +4925,16 @@
     </row>
     <row r="124">
       <c r="A124" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B124" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C124" t="s">
         <v>174</v>
       </c>
       <c r="D124" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="E124" t="s">
         <v>0</v>
@@ -4945,10 +4948,10 @@
     </row>
     <row r="125">
       <c r="A125" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B125" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C125" t="s">
         <v>23</v>
@@ -4968,14 +4971,14 @@
     </row>
     <row r="126">
       <c r="A126" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B126"/>
       <c r="C126" t="s">
         <v>194</v>
       </c>
       <c r="D126" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="E126" t="s">
         <v>0</v>
@@ -4989,10 +4992,10 @@
     </row>
     <row r="127">
       <c r="A127" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B127" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C127" t="s">
         <v>23</v>
@@ -5007,21 +5010,21 @@
         <v>0</v>
       </c>
       <c r="G127" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B128" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C128" t="s">
         <v>23</v>
       </c>
       <c r="D128" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="E128" t="s">
         <v>0</v>
@@ -5035,16 +5038,16 @@
     </row>
     <row r="129">
       <c r="A129" t="s">
+        <v>388</v>
+      </c>
+      <c r="B129" t="s">
+        <v>389</v>
+      </c>
+      <c r="C129" t="s">
+        <v>208</v>
+      </c>
+      <c r="D129" t="s">
         <v>390</v>
-      </c>
-      <c r="B129" t="s">
-        <v>391</v>
-      </c>
-      <c r="C129" t="s">
-        <v>209</v>
-      </c>
-      <c r="D129" t="s">
-        <v>392</v>
       </c>
       <c r="E129" t="s">
         <v>0</v>
@@ -5058,16 +5061,16 @@
     </row>
     <row r="130">
       <c r="A130" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B130" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C130" t="s">
         <v>160</v>
       </c>
       <c r="D130" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="E130" t="s">
         <v>0</v>
@@ -5081,16 +5084,16 @@
     </row>
     <row r="131">
       <c r="A131" t="s">
+        <v>394</v>
+      </c>
+      <c r="B131" t="s">
+        <v>395</v>
+      </c>
+      <c r="C131" t="s">
         <v>396</v>
       </c>
-      <c r="B131" t="s">
+      <c r="D131" t="s">
         <v>397</v>
-      </c>
-      <c r="C131" t="s">
-        <v>398</v>
-      </c>
-      <c r="D131" t="s">
-        <v>399</v>
       </c>
       <c r="E131" t="s">
         <v>0</v>
@@ -5104,10 +5107,10 @@
     </row>
     <row r="132">
       <c r="A132" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B132" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C132" t="s">
         <v>23</v>
@@ -5127,10 +5130,10 @@
     </row>
     <row r="133">
       <c r="A133" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B133" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C133" t="s">
         <v>23</v>
@@ -5150,16 +5153,16 @@
     </row>
     <row r="134">
       <c r="A134" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B134" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C134" t="s">
         <v>171</v>
       </c>
       <c r="D134" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E134" t="s">
         <v>0</v>
@@ -5173,16 +5176,16 @@
     </row>
     <row r="135">
       <c r="A135" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B135" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C135" t="s">
         <v>23</v>
       </c>
       <c r="D135" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="E135" t="s">
         <v>0</v>
@@ -5196,10 +5199,10 @@
     </row>
     <row r="136">
       <c r="A136" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B136" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C136" t="s">
         <v>23</v>
@@ -5219,14 +5222,14 @@
     </row>
     <row r="137">
       <c r="A137" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B137"/>
       <c r="C137" t="s">
         <v>194</v>
       </c>
       <c r="D137" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="E137" t="s">
         <v>0</v>
@@ -5240,19 +5243,19 @@
     </row>
     <row r="138">
       <c r="A138" t="s">
+        <v>411</v>
+      </c>
+      <c r="B138" t="s">
+        <v>211</v>
+      </c>
+      <c r="C138" t="s">
+        <v>412</v>
+      </c>
+      <c r="D138" t="s">
         <v>413</v>
       </c>
-      <c r="B138" t="s">
-        <v>212</v>
-      </c>
-      <c r="C138" t="s">
+      <c r="E138" t="s">
         <v>414</v>
-      </c>
-      <c r="D138" t="s">
-        <v>415</v>
-      </c>
-      <c r="E138" t="s">
-        <v>416</v>
       </c>
       <c r="F138" t="s">
         <v>0</v>
@@ -5263,16 +5266,16 @@
     </row>
     <row r="139">
       <c r="A139" t="s">
+        <v>415</v>
+      </c>
+      <c r="B139" t="s">
+        <v>238</v>
+      </c>
+      <c r="C139" t="s">
+        <v>416</v>
+      </c>
+      <c r="D139" t="s">
         <v>417</v>
-      </c>
-      <c r="B139" t="s">
-        <v>240</v>
-      </c>
-      <c r="C139" t="s">
-        <v>418</v>
-      </c>
-      <c r="D139" t="s">
-        <v>419</v>
       </c>
       <c r="E139" t="s">
         <v>0</v>
@@ -5286,7 +5289,7 @@
     </row>
     <row r="140">
       <c r="A140" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B140" t="s">
         <v>6</v>
@@ -5309,16 +5312,16 @@
     </row>
     <row r="141">
       <c r="A141" t="s">
+        <v>419</v>
+      </c>
+      <c r="B141" t="s">
+        <v>420</v>
+      </c>
+      <c r="C141" t="s">
         <v>421</v>
       </c>
-      <c r="B141" t="s">
+      <c r="D141" t="s">
         <v>422</v>
-      </c>
-      <c r="C141" t="s">
-        <v>423</v>
-      </c>
-      <c r="D141" t="s">
-        <v>424</v>
       </c>
       <c r="E141" t="s">
         <v>0</v>
@@ -5332,16 +5335,16 @@
     </row>
     <row r="142">
       <c r="A142" t="s">
+        <v>423</v>
+      </c>
+      <c r="B142" t="s">
+        <v>424</v>
+      </c>
+      <c r="C142" t="s">
         <v>425</v>
       </c>
-      <c r="B142" t="s">
+      <c r="D142" t="s">
         <v>426</v>
-      </c>
-      <c r="C142" t="s">
-        <v>427</v>
-      </c>
-      <c r="D142" t="s">
-        <v>428</v>
       </c>
       <c r="E142" t="s">
         <v>0</v>
@@ -5355,10 +5358,10 @@
     </row>
     <row r="143">
       <c r="A143" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="B143" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C143" t="s">
         <v>23</v>
@@ -5378,16 +5381,16 @@
     </row>
     <row r="144">
       <c r="A144" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B144" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C144" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D144" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="E144" t="s">
         <v>0</v>
@@ -5401,16 +5404,16 @@
     </row>
     <row r="145">
       <c r="A145" t="s">
+        <v>431</v>
+      </c>
+      <c r="B145" t="s">
+        <v>238</v>
+      </c>
+      <c r="C145" t="s">
+        <v>432</v>
+      </c>
+      <c r="D145" t="s">
         <v>433</v>
-      </c>
-      <c r="B145" t="s">
-        <v>240</v>
-      </c>
-      <c r="C145" t="s">
-        <v>434</v>
-      </c>
-      <c r="D145" t="s">
-        <v>435</v>
       </c>
       <c r="E145" t="s">
         <v>0</v>
@@ -5424,39 +5427,39 @@
     </row>
     <row r="146">
       <c r="A146" t="s">
+        <v>434</v>
+      </c>
+      <c r="B146" t="s">
+        <v>234</v>
+      </c>
+      <c r="C146" t="s">
+        <v>435</v>
+      </c>
+      <c r="D146" t="s">
         <v>436</v>
       </c>
-      <c r="B146" t="s">
-        <v>236</v>
-      </c>
-      <c r="C146" t="s">
+      <c r="E146" t="s">
         <v>437</v>
       </c>
-      <c r="D146" t="s">
-        <v>438</v>
-      </c>
-      <c r="E146" t="s">
-        <v>439</v>
-      </c>
       <c r="F146" t="s">
         <v>0</v>
       </c>
       <c r="G146" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="s">
+        <v>438</v>
+      </c>
+      <c r="B147" t="s">
+        <v>238</v>
+      </c>
+      <c r="C147" t="s">
+        <v>439</v>
+      </c>
+      <c r="D147" t="s">
         <v>440</v>
-      </c>
-      <c r="B147" t="s">
-        <v>240</v>
-      </c>
-      <c r="C147" t="s">
-        <v>441</v>
-      </c>
-      <c r="D147" t="s">
-        <v>442</v>
       </c>
       <c r="E147" t="s">
         <v>0</v>
@@ -5470,14 +5473,14 @@
     </row>
     <row r="148">
       <c r="A148" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B148"/>
       <c r="C148" t="s">
         <v>23</v>
       </c>
       <c r="D148" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E148" t="s">
         <v>0</v>
@@ -5491,10 +5494,10 @@
     </row>
     <row r="149">
       <c r="A149" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B149" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C149" t="s">
         <v>23</v>
@@ -5509,21 +5512,21 @@
         <v>0</v>
       </c>
       <c r="G149" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="s">
+        <v>445</v>
+      </c>
+      <c r="B150" t="s">
+        <v>446</v>
+      </c>
+      <c r="C150" t="s">
         <v>447</v>
       </c>
-      <c r="B150" t="s">
+      <c r="D150" t="s">
         <v>448</v>
-      </c>
-      <c r="C150" t="s">
-        <v>449</v>
-      </c>
-      <c r="D150" t="s">
-        <v>450</v>
       </c>
       <c r="E150" t="s">
         <v>0</v>
@@ -5537,16 +5540,16 @@
     </row>
     <row r="151">
       <c r="A151" t="s">
+        <v>449</v>
+      </c>
+      <c r="B151" t="s">
+        <v>450</v>
+      </c>
+      <c r="C151" t="s">
         <v>451</v>
       </c>
-      <c r="B151" t="s">
+      <c r="D151" t="s">
         <v>452</v>
-      </c>
-      <c r="C151" t="s">
-        <v>453</v>
-      </c>
-      <c r="D151" t="s">
-        <v>454</v>
       </c>
       <c r="E151" t="s">
         <v>0</v>
@@ -5560,7 +5563,7 @@
     </row>
     <row r="152">
       <c r="A152" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="B152"/>
       <c r="C152" t="s">
@@ -5581,108 +5584,108 @@
     </row>
     <row r="153">
       <c r="A153" t="s">
+        <v>454</v>
+      </c>
+      <c r="B153" t="s">
+        <v>0</v>
+      </c>
+      <c r="C153" t="s">
+        <v>455</v>
+      </c>
+      <c r="D153" t="s">
         <v>456</v>
       </c>
-      <c r="B153" t="s">
-        <v>0</v>
-      </c>
-      <c r="C153" t="s">
+      <c r="E153" t="s">
         <v>457</v>
       </c>
-      <c r="D153" t="s">
+      <c r="F153" t="s">
+        <v>0</v>
+      </c>
+      <c r="G153" t="s">
         <v>458</v>
-      </c>
-      <c r="E153" t="s">
-        <v>459</v>
-      </c>
-      <c r="F153" t="s">
-        <v>0</v>
-      </c>
-      <c r="G153" t="s">
-        <v>460</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="s">
+        <v>459</v>
+      </c>
+      <c r="B154" t="s">
+        <v>0</v>
+      </c>
+      <c r="C154" t="s">
+        <v>460</v>
+      </c>
+      <c r="D154" t="s">
         <v>461</v>
       </c>
-      <c r="B154" t="s">
-        <v>0</v>
-      </c>
-      <c r="C154" t="s">
+      <c r="E154" t="s">
         <v>462</v>
       </c>
-      <c r="D154" t="s">
+      <c r="F154" t="s">
+        <v>0</v>
+      </c>
+      <c r="G154" t="s">
         <v>463</v>
-      </c>
-      <c r="E154" t="s">
-        <v>464</v>
-      </c>
-      <c r="F154" t="s">
-        <v>0</v>
-      </c>
-      <c r="G154" t="s">
-        <v>465</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="s">
+        <v>464</v>
+      </c>
+      <c r="B155" t="s">
+        <v>0</v>
+      </c>
+      <c r="C155" t="s">
+        <v>465</v>
+      </c>
+      <c r="D155" t="s">
         <v>466</v>
       </c>
-      <c r="B155" t="s">
-        <v>0</v>
-      </c>
-      <c r="C155" t="s">
+      <c r="E155" t="s">
         <v>467</v>
       </c>
-      <c r="D155" t="s">
+      <c r="F155" t="s">
+        <v>0</v>
+      </c>
+      <c r="G155" t="s">
         <v>468</v>
-      </c>
-      <c r="E155" t="s">
-        <v>469</v>
-      </c>
-      <c r="F155" t="s">
-        <v>0</v>
-      </c>
-      <c r="G155" t="s">
-        <v>470</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="s">
+        <v>469</v>
+      </c>
+      <c r="B156" t="s">
+        <v>470</v>
+      </c>
+      <c r="C156" t="s">
         <v>471</v>
       </c>
-      <c r="B156" t="s">
+      <c r="D156" t="s">
         <v>472</v>
       </c>
-      <c r="C156" t="s">
+      <c r="E156" t="s">
         <v>473</v>
       </c>
-      <c r="D156" t="s">
+      <c r="F156" t="s">
+        <v>0</v>
+      </c>
+      <c r="G156" t="s">
         <v>474</v>
-      </c>
-      <c r="E156" t="s">
-        <v>475</v>
-      </c>
-      <c r="F156" t="s">
-        <v>0</v>
-      </c>
-      <c r="G156" t="s">
-        <v>476</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="s">
+        <v>475</v>
+      </c>
+      <c r="B157" t="s">
+        <v>476</v>
+      </c>
+      <c r="C157" t="s">
         <v>477</v>
       </c>
-      <c r="B157" t="s">
+      <c r="D157" t="s">
         <v>478</v>
-      </c>
-      <c r="C157" t="s">
-        <v>479</v>
-      </c>
-      <c r="D157" t="s">
-        <v>480</v>
       </c>
       <c r="E157" t="s">
         <v>0</v>
@@ -5696,14 +5699,14 @@
     </row>
     <row r="158">
       <c r="A158" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="B158"/>
       <c r="C158" t="s">
         <v>171</v>
       </c>
       <c r="D158" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="E158" t="s">
         <v>0</v>
@@ -5717,39 +5720,39 @@
     </row>
     <row r="159">
       <c r="A159" t="s">
+        <v>481</v>
+      </c>
+      <c r="B159" t="s">
+        <v>470</v>
+      </c>
+      <c r="C159" t="s">
+        <v>229</v>
+      </c>
+      <c r="D159" t="s">
+        <v>482</v>
+      </c>
+      <c r="E159" t="s">
         <v>483</v>
       </c>
-      <c r="B159" t="s">
-        <v>472</v>
-      </c>
-      <c r="C159" t="s">
-        <v>231</v>
-      </c>
-      <c r="D159" t="s">
+      <c r="F159" t="s">
+        <v>0</v>
+      </c>
+      <c r="G159" t="s">
         <v>484</v>
-      </c>
-      <c r="E159" t="s">
-        <v>485</v>
-      </c>
-      <c r="F159" t="s">
-        <v>0</v>
-      </c>
-      <c r="G159" t="s">
-        <v>486</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="B160" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="C160" t="s">
         <v>95</v>
       </c>
       <c r="D160" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="E160" t="s">
         <v>0</v>
@@ -5763,14 +5766,14 @@
     </row>
     <row r="161">
       <c r="A161" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="B161"/>
       <c r="C161" t="s">
         <v>180</v>
       </c>
       <c r="D161" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="E161" t="s">
         <v>0</v>
@@ -5784,85 +5787,85 @@
     </row>
     <row r="162">
       <c r="A162" t="s">
+        <v>489</v>
+      </c>
+      <c r="B162" t="s">
+        <v>0</v>
+      </c>
+      <c r="C162" t="s">
+        <v>490</v>
+      </c>
+      <c r="D162" t="s">
         <v>491</v>
       </c>
-      <c r="B162" t="s">
-        <v>0</v>
-      </c>
-      <c r="C162" t="s">
+      <c r="E162" t="s">
         <v>492</v>
       </c>
-      <c r="D162" t="s">
+      <c r="F162" t="s">
+        <v>0</v>
+      </c>
+      <c r="G162" t="s">
         <v>493</v>
-      </c>
-      <c r="E162" t="s">
-        <v>494</v>
-      </c>
-      <c r="F162" t="s">
-        <v>0</v>
-      </c>
-      <c r="G162" t="s">
-        <v>495</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="s">
+        <v>494</v>
+      </c>
+      <c r="B163" t="s">
+        <v>0</v>
+      </c>
+      <c r="C163" t="s">
+        <v>495</v>
+      </c>
+      <c r="D163" t="s">
         <v>496</v>
       </c>
-      <c r="B163" t="s">
-        <v>0</v>
-      </c>
-      <c r="C163" t="s">
+      <c r="E163" t="s">
+        <v>142</v>
+      </c>
+      <c r="F163" t="s">
+        <v>0</v>
+      </c>
+      <c r="G163" t="s">
         <v>497</v>
-      </c>
-      <c r="D163" t="s">
-        <v>498</v>
-      </c>
-      <c r="E163" t="s">
-        <v>499</v>
-      </c>
-      <c r="F163" t="s">
-        <v>0</v>
-      </c>
-      <c r="G163" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="s">
+        <v>498</v>
+      </c>
+      <c r="B164" t="s">
+        <v>234</v>
+      </c>
+      <c r="C164" t="s">
+        <v>499</v>
+      </c>
+      <c r="D164" t="s">
+        <v>500</v>
+      </c>
+      <c r="E164" t="s">
         <v>501</v>
       </c>
-      <c r="B164" t="s">
-        <v>236</v>
-      </c>
-      <c r="C164" t="s">
+      <c r="F164" t="s">
+        <v>0</v>
+      </c>
+      <c r="G164" t="s">
         <v>502</v>
-      </c>
-      <c r="D164" t="s">
-        <v>503</v>
-      </c>
-      <c r="E164" t="s">
-        <v>504</v>
-      </c>
-      <c r="F164" t="s">
-        <v>0</v>
-      </c>
-      <c r="G164" t="s">
-        <v>505</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="B165" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C165" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="D165" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="E165" t="s">
         <v>0</v>
@@ -5876,14 +5879,14 @@
     </row>
     <row r="166">
       <c r="A166" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="B166"/>
       <c r="C166" t="s">
         <v>171</v>
       </c>
       <c r="D166" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="E166" t="s">
         <v>0</v>
@@ -5897,62 +5900,62 @@
     </row>
     <row r="167">
       <c r="A167" t="s">
+        <v>507</v>
+      </c>
+      <c r="B167" t="s">
+        <v>0</v>
+      </c>
+      <c r="C167" t="s">
+        <v>508</v>
+      </c>
+      <c r="D167" t="s">
+        <v>509</v>
+      </c>
+      <c r="E167" t="s">
         <v>510</v>
       </c>
-      <c r="B167" t="s">
-        <v>0</v>
-      </c>
-      <c r="C167" t="s">
+      <c r="F167" t="s">
+        <v>0</v>
+      </c>
+      <c r="G167" t="s">
         <v>511</v>
-      </c>
-      <c r="D167" t="s">
-        <v>512</v>
-      </c>
-      <c r="E167" t="s">
-        <v>513</v>
-      </c>
-      <c r="F167" t="s">
-        <v>0</v>
-      </c>
-      <c r="G167" t="s">
-        <v>514</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="s">
+        <v>512</v>
+      </c>
+      <c r="B168" t="s">
+        <v>470</v>
+      </c>
+      <c r="C168" t="s">
+        <v>499</v>
+      </c>
+      <c r="D168" t="s">
+        <v>513</v>
+      </c>
+      <c r="E168" t="s">
+        <v>514</v>
+      </c>
+      <c r="F168" t="s">
+        <v>0</v>
+      </c>
+      <c r="G168" t="s">
         <v>515</v>
-      </c>
-      <c r="B168" t="s">
-        <v>472</v>
-      </c>
-      <c r="C168" t="s">
-        <v>502</v>
-      </c>
-      <c r="D168" t="s">
-        <v>516</v>
-      </c>
-      <c r="E168" t="s">
-        <v>517</v>
-      </c>
-      <c r="F168" t="s">
-        <v>0</v>
-      </c>
-      <c r="G168" t="s">
-        <v>518</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="B169" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="C169" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="D169" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="E169" t="s">
         <v>0</v>
@@ -5966,14 +5969,14 @@
     </row>
     <row r="170">
       <c r="A170" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="B170"/>
       <c r="C170" t="s">
         <v>23</v>
       </c>
       <c r="D170" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="E170" t="s">
         <v>0</v>
@@ -5987,39 +5990,39 @@
     </row>
     <row r="171">
       <c r="A171" t="s">
+        <v>521</v>
+      </c>
+      <c r="B171" t="s">
+        <v>470</v>
+      </c>
+      <c r="C171" t="s">
+        <v>522</v>
+      </c>
+      <c r="D171" t="s">
+        <v>523</v>
+      </c>
+      <c r="E171" t="s">
         <v>524</v>
       </c>
-      <c r="B171" t="s">
-        <v>472</v>
-      </c>
-      <c r="C171" t="s">
-        <v>525</v>
-      </c>
-      <c r="D171" t="s">
-        <v>526</v>
-      </c>
-      <c r="E171" t="s">
-        <v>527</v>
-      </c>
       <c r="F171" t="s">
         <v>0</v>
       </c>
       <c r="G171" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="B172" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="C172" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="D172" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="E172" t="s">
         <v>0</v>
@@ -6033,14 +6036,14 @@
     </row>
     <row r="173">
       <c r="A173" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="B173"/>
       <c r="C173" t="s">
         <v>171</v>
       </c>
       <c r="D173" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="E173" t="s">
         <v>0</v>
@@ -6054,39 +6057,39 @@
     </row>
     <row r="174">
       <c r="A174" t="s">
+        <v>529</v>
+      </c>
+      <c r="B174" t="s">
+        <v>530</v>
+      </c>
+      <c r="C174" t="s">
+        <v>531</v>
+      </c>
+      <c r="D174" t="s">
         <v>532</v>
       </c>
-      <c r="B174" t="s">
+      <c r="E174" t="s">
         <v>533</v>
       </c>
-      <c r="C174" t="s">
+      <c r="F174" t="s">
+        <v>0</v>
+      </c>
+      <c r="G174" t="s">
         <v>534</v>
-      </c>
-      <c r="D174" t="s">
-        <v>535</v>
-      </c>
-      <c r="E174" t="s">
-        <v>536</v>
-      </c>
-      <c r="F174" t="s">
-        <v>0</v>
-      </c>
-      <c r="G174" t="s">
-        <v>537</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="s">
+        <v>535</v>
+      </c>
+      <c r="B175" t="s">
+        <v>536</v>
+      </c>
+      <c r="C175" t="s">
+        <v>537</v>
+      </c>
+      <c r="D175" t="s">
         <v>538</v>
-      </c>
-      <c r="B175" t="s">
-        <v>539</v>
-      </c>
-      <c r="C175" t="s">
-        <v>540</v>
-      </c>
-      <c r="D175" t="s">
-        <v>541</v>
       </c>
       <c r="E175" t="s">
         <v>0</v>
@@ -6100,14 +6103,14 @@
     </row>
     <row r="176">
       <c r="A176" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="B176"/>
       <c r="C176" t="s">
         <v>23</v>
       </c>
       <c r="D176" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="E176" t="s">
         <v>0</v>
@@ -6121,39 +6124,39 @@
     </row>
     <row r="177">
       <c r="A177" t="s">
+        <v>541</v>
+      </c>
+      <c r="B177" t="s">
+        <v>542</v>
+      </c>
+      <c r="C177" t="s">
+        <v>224</v>
+      </c>
+      <c r="D177" t="s">
+        <v>543</v>
+      </c>
+      <c r="E177" t="s">
         <v>544</v>
       </c>
-      <c r="B177" t="s">
-        <v>545</v>
-      </c>
-      <c r="C177" t="s">
-        <v>226</v>
-      </c>
-      <c r="D177" t="s">
-        <v>546</v>
-      </c>
-      <c r="E177" t="s">
-        <v>547</v>
-      </c>
       <c r="F177" t="s">
         <v>0</v>
       </c>
       <c r="G177" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="B178" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="C178" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D178" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="E178" t="s">
         <v>0</v>
@@ -6167,14 +6170,14 @@
     </row>
     <row r="179">
       <c r="A179" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="B179"/>
       <c r="C179" t="s">
         <v>23</v>
       </c>
       <c r="D179" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="E179" t="s">
         <v>0</v>
@@ -6188,39 +6191,39 @@
     </row>
     <row r="180">
       <c r="A180" t="s">
+        <v>549</v>
+      </c>
+      <c r="B180" t="s">
+        <v>550</v>
+      </c>
+      <c r="C180" t="s">
+        <v>551</v>
+      </c>
+      <c r="D180" t="s">
         <v>552</v>
       </c>
-      <c r="B180" t="s">
+      <c r="E180" t="s">
         <v>553</v>
       </c>
-      <c r="C180" t="s">
-        <v>554</v>
-      </c>
-      <c r="D180" t="s">
-        <v>555</v>
-      </c>
-      <c r="E180" t="s">
-        <v>556</v>
-      </c>
       <c r="F180" t="s">
         <v>0</v>
       </c>
       <c r="G180" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="B181" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="C181" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="D181" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="E181" t="s">
         <v>0</v>
@@ -6234,16 +6237,16 @@
     </row>
     <row r="182">
       <c r="A182" t="s">
+        <v>557</v>
+      </c>
+      <c r="B182" t="s">
+        <v>558</v>
+      </c>
+      <c r="C182" t="s">
+        <v>559</v>
+      </c>
+      <c r="D182" t="s">
         <v>560</v>
-      </c>
-      <c r="B182" t="s">
-        <v>561</v>
-      </c>
-      <c r="C182" t="s">
-        <v>562</v>
-      </c>
-      <c r="D182" t="s">
-        <v>563</v>
       </c>
       <c r="E182" t="s">
         <v>0</v>
@@ -6257,7 +6260,7 @@
     </row>
     <row r="183">
       <c r="A183" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="B183"/>
       <c r="C183" t="s">
@@ -6278,117 +6281,140 @@
     </row>
     <row r="184">
       <c r="A184" t="s">
+        <v>562</v>
+      </c>
+      <c r="B184" t="s">
+        <v>0</v>
+      </c>
+      <c r="C184" t="s">
+        <v>563</v>
+      </c>
+      <c r="D184" t="s">
+        <v>564</v>
+      </c>
+      <c r="E184" t="s">
         <v>565</v>
       </c>
-      <c r="B184" t="s">
-        <v>0</v>
-      </c>
-      <c r="C184" t="s">
+      <c r="F184" t="s">
+        <v>0</v>
+      </c>
+      <c r="G184" t="s">
         <v>566</v>
-      </c>
-      <c r="D184" t="s">
-        <v>567</v>
-      </c>
-      <c r="E184" t="s">
-        <v>568</v>
-      </c>
-      <c r="F184" t="s">
-        <v>0</v>
-      </c>
-      <c r="G184" t="s">
-        <v>569</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="s">
+        <v>567</v>
+      </c>
+      <c r="B185" t="s">
+        <v>0</v>
+      </c>
+      <c r="C185" t="s">
+        <v>568</v>
+      </c>
+      <c r="D185" t="s">
+        <v>569</v>
+      </c>
+      <c r="E185" t="s">
         <v>570</v>
       </c>
-      <c r="B185" t="s">
-        <v>0</v>
-      </c>
-      <c r="C185" t="s">
+      <c r="F185" t="s">
+        <v>0</v>
+      </c>
+      <c r="G185" t="s">
         <v>571</v>
-      </c>
-      <c r="D185" t="s">
-        <v>572</v>
-      </c>
-      <c r="E185" t="s">
-        <v>573</v>
-      </c>
-      <c r="F185" t="s">
-        <v>0</v>
-      </c>
-      <c r="G185" t="s">
-        <v>574</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="s">
+        <v>572</v>
+      </c>
+      <c r="B186" t="s">
+        <v>0</v>
+      </c>
+      <c r="C186" t="s">
+        <v>573</v>
+      </c>
+      <c r="D186" t="s">
+        <v>574</v>
+      </c>
+      <c r="E186" t="s">
         <v>575</v>
       </c>
-      <c r="B186" t="s">
-        <v>0</v>
-      </c>
-      <c r="C186" t="s">
+      <c r="F186" t="s">
+        <v>0</v>
+      </c>
+      <c r="G186" t="s">
         <v>576</v>
-      </c>
-      <c r="D186" t="s">
-        <v>577</v>
-      </c>
-      <c r="E186" t="s">
-        <v>578</v>
-      </c>
-      <c r="F186" t="s">
-        <v>0</v>
-      </c>
-      <c r="G186" t="s">
-        <v>579</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="s">
+        <v>577</v>
+      </c>
+      <c r="B187" t="s">
+        <v>0</v>
+      </c>
+      <c r="C187" t="s">
+        <v>578</v>
+      </c>
+      <c r="D187" t="s">
+        <v>579</v>
+      </c>
+      <c r="E187" t="s">
         <v>580</v>
       </c>
-      <c r="B187" t="s">
-        <v>0</v>
-      </c>
-      <c r="C187" t="s">
+      <c r="F187" t="s">
+        <v>0</v>
+      </c>
+      <c r="G187" t="s">
         <v>581</v>
-      </c>
-      <c r="D187" t="s">
-        <v>582</v>
-      </c>
-      <c r="E187" t="s">
-        <v>583</v>
-      </c>
-      <c r="F187" t="s">
-        <v>0</v>
-      </c>
-      <c r="G187" t="s">
-        <v>584</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="s">
+        <v>582</v>
+      </c>
+      <c r="B188" t="s">
+        <v>0</v>
+      </c>
+      <c r="C188" t="s">
+        <v>583</v>
+      </c>
+      <c r="D188" t="s">
+        <v>584</v>
+      </c>
+      <c r="E188" t="s">
         <v>585</v>
       </c>
-      <c r="B188" t="s">
-        <v>0</v>
-      </c>
-      <c r="C188" t="s">
+      <c r="F188" t="s">
+        <v>0</v>
+      </c>
+      <c r="G188" t="s">
         <v>586</v>
       </c>
-      <c r="D188" t="s">
+    </row>
+    <row r="189">
+      <c r="A189" t="s">
         <v>587</v>
       </c>
-      <c r="E188" t="s">
+      <c r="B189" t="s">
+        <v>0</v>
+      </c>
+      <c r="C189" t="s">
         <v>588</v>
       </c>
-      <c r="F188" t="s">
-        <v>0</v>
-      </c>
-      <c r="G188" t="s">
+      <c r="D189" t="s">
         <v>589</v>
+      </c>
+      <c r="E189" t="s">
+        <v>590</v>
+      </c>
+      <c r="F189" t="s">
+        <v>0</v>
+      </c>
+      <c r="G189" t="s">
+        <v>586</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
* v1.0.18 Changed 'asymptomatic vs. symptomatic DotPlot to have dots instead of lines.
</commit_message>
<xml_diff>
--- a/IL6MCP1/BASELINE/20200625.IL6MCP1.AE.BaselineTable.subsetCEA.xlsx
+++ b/IL6MCP1/BASELINE/20200625.IL6MCP1.AE.BaselineTable.subsetCEA.xlsx
@@ -1,41 +1,49 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/swvanderlaan/PLINK/analyses/lookups/AE_20190912_010_MDICHGANS_SWVDLAAN_IL6_MCP1/IL6MCP1/BASELINE/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{450491AF-5148-AC4E-BF5B-EA4C3DB27E49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="13120" windowHeight="6100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="subsetAEDB_Baseline" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="subsetAEDB_Baseline" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="591">
-  <si>
-    <t xml:space="preserve"/>
-  </si>
-  <si>
-    <t xml:space="preserve">level</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Asymptomatic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Symptomatic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">p</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Missing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">n</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1300" uniqueCount="591">
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>level</t>
+  </si>
+  <si>
+    <t>Asymptomatic</t>
+  </si>
+  <si>
+    <t>Symptomatic</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>Missing</t>
+  </si>
+  <si>
+    <t>n</t>
   </si>
   <si>
     <t xml:space="preserve">    161</t>
@@ -47,10 +55,10 @@
     <t xml:space="preserve">    </t>
   </si>
   <si>
-    <t xml:space="preserve">Hospital....freq.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">St. Antonius, Nieuwegein</t>
+    <t>Hospital....freq.</t>
+  </si>
+  <si>
+    <t>St. Antonius, Nieuwegein</t>
   </si>
   <si>
     <t xml:space="preserve">   52.2 ( 84) </t>
@@ -65,10 +73,10 @@
     <t xml:space="preserve"> 0.0</t>
   </si>
   <si>
-    <t xml:space="preserve">X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UMC Utrecht</t>
+    <t>X</t>
+  </si>
+  <si>
+    <t>UMC Utrecht</t>
   </si>
   <si>
     <t xml:space="preserve">   47.8 ( 77) </t>
@@ -77,10 +85,10 @@
     <t xml:space="preserve">   53.1 ( 620) </t>
   </si>
   <si>
-    <t xml:space="preserve">ORyear....freq.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No data available/missing</t>
+    <t>ORyear....freq.</t>
+  </si>
+  <si>
+    <t>No data available/missing</t>
   </si>
   <si>
     <t xml:space="preserve">    0.0 (  0) </t>
@@ -92,10 +100,10 @@
     <t xml:space="preserve"> NaN</t>
   </si>
   <si>
-    <t xml:space="preserve">X.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2002</t>
+    <t>X.1</t>
+  </si>
+  <si>
+    <t>2002</t>
   </si>
   <si>
     <t xml:space="preserve">   10.6 ( 17) </t>
@@ -104,10 +112,10 @@
     <t xml:space="preserve">    4.8 (  56) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2003</t>
+    <t>X.2</t>
+  </si>
+  <si>
+    <t>2003</t>
   </si>
   <si>
     <t xml:space="preserve">   11.8 ( 19) </t>
@@ -116,10 +124,10 @@
     <t xml:space="preserve">   10.6 ( 124) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2004</t>
+    <t>X.3</t>
+  </si>
+  <si>
+    <t>2004</t>
   </si>
   <si>
     <t xml:space="preserve">   19.9 ( 32) </t>
@@ -128,10 +136,10 @@
     <t xml:space="preserve">   12.2 ( 142) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2005</t>
+    <t>X.4</t>
+  </si>
+  <si>
+    <t>2005</t>
   </si>
   <si>
     <t xml:space="preserve">   13.7 ( 22) </t>
@@ -140,10 +148,10 @@
     <t xml:space="preserve">   13.3 ( 155) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2006</t>
+    <t>X.5</t>
+  </si>
+  <si>
+    <t>2006</t>
   </si>
   <si>
     <t xml:space="preserve">    8.7 ( 14) </t>
@@ -152,10 +160,10 @@
     <t xml:space="preserve">    9.9 ( 116) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2007</t>
+    <t>X.6</t>
+  </si>
+  <si>
+    <t>2007</t>
   </si>
   <si>
     <t xml:space="preserve">    9.3 ( 15) </t>
@@ -164,10 +172,10 @@
     <t xml:space="preserve">    9.6 ( 112) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2008</t>
+    <t>X.7</t>
+  </si>
+  <si>
+    <t>2008</t>
   </si>
   <si>
     <t xml:space="preserve">    6.2 ( 10) </t>
@@ -176,19 +184,19 @@
     <t xml:space="preserve">    6.8 (  79) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2009</t>
+    <t>X.8</t>
+  </si>
+  <si>
+    <t>2009</t>
   </si>
   <si>
     <t xml:space="preserve">    7.7 (  90) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2010</t>
+    <t>X.9</t>
+  </si>
+  <si>
+    <t>2010</t>
   </si>
   <si>
     <t xml:space="preserve">    4.3 (  7) </t>
@@ -197,10 +205,10 @@
     <t xml:space="preserve">    6.9 (  81) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2011</t>
+    <t>X.10</t>
+  </si>
+  <si>
+    <t>2011</t>
   </si>
   <si>
     <t xml:space="preserve">    5.0 (  8) </t>
@@ -209,64 +217,64 @@
     <t xml:space="preserve">    8.7 ( 102) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2012</t>
+    <t>X.11</t>
+  </si>
+  <si>
+    <t>2012</t>
   </si>
   <si>
     <t xml:space="preserve">    7.5 (  88) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2013</t>
+    <t>X.12</t>
+  </si>
+  <si>
+    <t>2013</t>
   </si>
   <si>
     <t xml:space="preserve">    1.8 (  21) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2014</t>
+    <t>X.13</t>
+  </si>
+  <si>
+    <t>2014</t>
   </si>
   <si>
     <t xml:space="preserve">    0.1 (   1) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Age..mean..SD..</t>
+    <t>X.14</t>
+  </si>
+  <si>
+    <t>2015</t>
+  </si>
+  <si>
+    <t>X.15</t>
+  </si>
+  <si>
+    <t>2016</t>
+  </si>
+  <si>
+    <t>X.16</t>
+  </si>
+  <si>
+    <t>2017</t>
+  </si>
+  <si>
+    <t>X.17</t>
+  </si>
+  <si>
+    <t>2018</t>
+  </si>
+  <si>
+    <t>X.18</t>
+  </si>
+  <si>
+    <t>2019</t>
+  </si>
+  <si>
+    <t>Age..mean..SD..</t>
   </si>
   <si>
     <t xml:space="preserve"> 65.901 (9.051)</t>
@@ -275,13 +283,13 @@
     <t xml:space="preserve"> 68.785 (9.081)</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;0.001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gender....freq.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">female</t>
+    <t>&lt;0.001</t>
+  </si>
+  <si>
+    <t>Gender....freq.</t>
+  </si>
+  <si>
+    <t>female</t>
   </si>
   <si>
     <t xml:space="preserve">   23.0 ( 37) </t>
@@ -293,10 +301,10 @@
     <t xml:space="preserve"> 0.065</t>
   </si>
   <si>
-    <t xml:space="preserve">X.19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">male</t>
+    <t>X.19</t>
+  </si>
+  <si>
+    <t>male</t>
   </si>
   <si>
     <t xml:space="preserve">   77.0 (124) </t>
@@ -305,37 +313,37 @@
     <t xml:space="preserve">   69.6 ( 812) </t>
   </si>
   <si>
-    <t xml:space="preserve">TC_finalCU..mean..SD..</t>
-  </si>
-  <si>
-    <t xml:space="preserve">179.199 (45.274)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">184.078 (48.333)</t>
+    <t>TC_finalCU..mean..SD..</t>
+  </si>
+  <si>
+    <t>179.199 (45.274)</t>
+  </si>
+  <si>
+    <t>184.078 (48.333)</t>
   </si>
   <si>
     <t xml:space="preserve"> 0.322</t>
   </si>
   <si>
-    <t xml:space="preserve">32.8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LDL_finalCU..mean..SD..</t>
-  </si>
-  <si>
-    <t xml:space="preserve">104.132 (37.590)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">109.761 (41.318)</t>
+    <t>32.8</t>
+  </si>
+  <si>
+    <t>LDL_finalCU..mean..SD..</t>
+  </si>
+  <si>
+    <t>104.132 (37.590)</t>
+  </si>
+  <si>
+    <t>109.761 (41.318)</t>
   </si>
   <si>
     <t xml:space="preserve"> 0.206</t>
   </si>
   <si>
-    <t xml:space="preserve">39.8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HDL_finalCU..mean..SD..</t>
+    <t>39.8</t>
+  </si>
+  <si>
+    <t>HDL_finalCU..mean..SD..</t>
   </si>
   <si>
     <t xml:space="preserve"> 44.749 (14.890)</t>
@@ -347,25 +355,25 @@
     <t xml:space="preserve"> 0.570</t>
   </si>
   <si>
-    <t xml:space="preserve">36.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TG_finalCU..mean..SD..</t>
-  </si>
-  <si>
-    <t xml:space="preserve">158.699 (87.584)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">145.901 (83.176)</t>
+    <t>36.1</t>
+  </si>
+  <si>
+    <t>TG_finalCU..mean..SD..</t>
+  </si>
+  <si>
+    <t>158.699 (87.584)</t>
+  </si>
+  <si>
+    <t>145.901 (83.176)</t>
   </si>
   <si>
     <t xml:space="preserve"> 0.141</t>
   </si>
   <si>
-    <t xml:space="preserve">35.6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_final..mean..SD..</t>
+    <t>35.6</t>
+  </si>
+  <si>
+    <t>TC_final..mean..SD..</t>
   </si>
   <si>
     <t xml:space="preserve">  4.641 (1.173)</t>
@@ -374,7 +382,7 @@
     <t xml:space="preserve">  4.768 (1.252)</t>
   </si>
   <si>
-    <t xml:space="preserve">LDL_final..mean..SD..</t>
+    <t>LDL_final..mean..SD..</t>
   </si>
   <si>
     <t xml:space="preserve">  2.697 (0.974)</t>
@@ -383,7 +391,7 @@
     <t xml:space="preserve">  2.843 (1.070)</t>
   </si>
   <si>
-    <t xml:space="preserve">HDL_final..mean..SD..</t>
+    <t>HDL_final..mean..SD..</t>
   </si>
   <si>
     <t xml:space="preserve">  1.159 (0.386)</t>
@@ -392,7 +400,7 @@
     <t xml:space="preserve">  1.186 (0.472)</t>
   </si>
   <si>
-    <t xml:space="preserve">TG_final..mean..SD..</t>
+    <t>TG_final..mean..SD..</t>
   </si>
   <si>
     <t xml:space="preserve">  1.793 (0.990)</t>
@@ -401,7 +409,7 @@
     <t xml:space="preserve">  1.649 (0.940)</t>
   </si>
   <si>
-    <t xml:space="preserve">hsCRP_plasma..mean..SD..</t>
+    <t>hsCRP_plasma..mean..SD..</t>
   </si>
   <si>
     <t xml:space="preserve">  6.846 (21.838)</t>
@@ -413,25 +421,25 @@
     <t xml:space="preserve"> 0.394</t>
   </si>
   <si>
-    <t xml:space="preserve">40.6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">systolic..mean..SD..</t>
-  </si>
-  <si>
-    <t xml:space="preserve">152.838 (24.600)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">155.713 (26.406)</t>
+    <t>40.6</t>
+  </si>
+  <si>
+    <t>systolic..mean..SD..</t>
+  </si>
+  <si>
+    <t>152.838 (24.600)</t>
+  </si>
+  <si>
+    <t>155.713 (26.406)</t>
   </si>
   <si>
     <t xml:space="preserve"> 0.230</t>
   </si>
   <si>
-    <t xml:space="preserve">13.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diastoli..mean..SD..</t>
+    <t>13.5</t>
+  </si>
+  <si>
+    <t>diastoli..mean..SD..</t>
   </si>
   <si>
     <t xml:space="preserve"> 80.824 (12.855)</t>
@@ -443,7 +451,7 @@
     <t xml:space="preserve"> 0.097</t>
   </si>
   <si>
-    <t xml:space="preserve">GFR_MDRD..mean..SD..</t>
+    <t>GFR_MDRD..mean..SD..</t>
   </si>
   <si>
     <t xml:space="preserve"> 70.440 (19.793)</t>
@@ -458,7 +466,7 @@
     <t xml:space="preserve"> 3.5</t>
   </si>
   <si>
-    <t xml:space="preserve">BMI..mean..SD..</t>
+    <t>BMI..mean..SD..</t>
   </si>
   <si>
     <t xml:space="preserve"> 26.626 (3.572)</t>
@@ -473,13 +481,13 @@
     <t xml:space="preserve"> 4.4</t>
   </si>
   <si>
-    <t xml:space="preserve">KDOQI....freq.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Normal kidney function</t>
+    <t>KDOQI....freq.</t>
+  </si>
+  <si>
+    <t>X.20</t>
+  </si>
+  <si>
+    <t>Normal kidney function</t>
   </si>
   <si>
     <t xml:space="preserve">   14.9 ( 24) </t>
@@ -488,10 +496,10 @@
     <t xml:space="preserve">   17.4 ( 203) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CKD 2 (Mild)</t>
+    <t>X.21</t>
+  </si>
+  <si>
+    <t>CKD 2 (Mild)</t>
   </si>
   <si>
     <t xml:space="preserve">   50.9 ( 82) </t>
@@ -500,10 +508,10 @@
     <t xml:space="preserve">   53.4 ( 623) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CKD 3 (Moderate)</t>
+    <t>X.22</t>
+  </si>
+  <si>
+    <t>CKD 3 (Moderate)</t>
   </si>
   <si>
     <t xml:space="preserve">   29.8 ( 48) </t>
@@ -512,19 +520,19 @@
     <t xml:space="preserve">   24.0 ( 280) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CKD 4 (Severe)</t>
+    <t>X.23</t>
+  </si>
+  <si>
+    <t>CKD 4 (Severe)</t>
   </si>
   <si>
     <t xml:space="preserve">    1.3 (  15) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CKD 5 (Failure)</t>
+    <t>X.24</t>
+  </si>
+  <si>
+    <t>CKD 5 (Failure)</t>
   </si>
   <si>
     <t xml:space="preserve">    0.6 (  1) </t>
@@ -533,7 +541,7 @@
     <t xml:space="preserve">    0.4 (   5) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.25</t>
+    <t>X.25</t>
   </si>
   <si>
     <t xml:space="preserve">    3.7 (  6) </t>
@@ -542,16 +550,16 @@
     <t xml:space="preserve">    3.5 (  41) </t>
   </si>
   <si>
-    <t xml:space="preserve">BMI_WHO....freq.</t>
+    <t>BMI_WHO....freq.</t>
   </si>
   <si>
     <t xml:space="preserve"> 4.6</t>
   </si>
   <si>
-    <t xml:space="preserve">X.26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Underweight</t>
+    <t>X.26</t>
+  </si>
+  <si>
+    <t>Underweight</t>
   </si>
   <si>
     <t xml:space="preserve">    1.2 (  2) </t>
@@ -560,10 +568,10 @@
     <t xml:space="preserve">    0.9 (  11) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Normal</t>
+    <t>X.27</t>
+  </si>
+  <si>
+    <t>Normal</t>
   </si>
   <si>
     <t xml:space="preserve">   32.3 ( 52) </t>
@@ -572,10 +580,10 @@
     <t xml:space="preserve">   35.6 ( 415) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.28</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Overweight</t>
+    <t>X.28</t>
+  </si>
+  <si>
+    <t>Overweight</t>
   </si>
   <si>
     <t xml:space="preserve">   49.7 ( 80) </t>
@@ -584,25 +592,25 @@
     <t xml:space="preserve">   45.6 ( 532) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.29</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Obese</t>
+    <t>X.29</t>
+  </si>
+  <si>
+    <t>Obese</t>
   </si>
   <si>
     <t xml:space="preserve">   13.1 ( 153) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.30</t>
+    <t>X.30</t>
   </si>
   <si>
     <t xml:space="preserve">    3.1 (  5) </t>
   </si>
   <si>
-    <t xml:space="preserve">SmokerStatus....freq.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Current smoker</t>
+    <t>SmokerStatus....freq.</t>
+  </si>
+  <si>
+    <t>Current smoker</t>
   </si>
   <si>
     <t xml:space="preserve">   29.2 ( 47) </t>
@@ -617,25 +625,25 @@
     <t xml:space="preserve"> 4.0</t>
   </si>
   <si>
-    <t xml:space="preserve">X.31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ex-smoker</t>
+    <t>X.31</t>
+  </si>
+  <si>
+    <t>Ex-smoker</t>
   </si>
   <si>
     <t xml:space="preserve">   56.5 ( 91) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.32</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Never smoked</t>
+    <t>X.32</t>
+  </si>
+  <si>
+    <t>Never smoked</t>
   </si>
   <si>
     <t xml:space="preserve">   14.1 ( 165) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.33</t>
+    <t>X.33</t>
   </si>
   <si>
     <t xml:space="preserve">    2.5 (  4) </t>
@@ -644,10 +652,10 @@
     <t xml:space="preserve">    4.2 (  49) </t>
   </si>
   <si>
-    <t xml:space="preserve">AlcoholUse....freq.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No</t>
+    <t>AlcoholUse....freq.</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
   <si>
     <t xml:space="preserve">   38.5 ( 62) </t>
@@ -662,10 +670,10 @@
     <t xml:space="preserve"> 3.9</t>
   </si>
   <si>
-    <t xml:space="preserve">X.34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes</t>
+    <t>X.34</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
   <si>
     <t xml:space="preserve">   59.6 ( 96) </t>
@@ -674,16 +682,16 @@
     <t xml:space="preserve">   62.2 ( 726) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.35</t>
+    <t>X.35</t>
   </si>
   <si>
     <t xml:space="preserve">    1.9 (  3) </t>
   </si>
   <si>
-    <t xml:space="preserve">DiabetesStatus....freq.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Control (no Diabetes Dx/Med)</t>
+    <t>DiabetesStatus....freq.</t>
+  </si>
+  <si>
+    <t>Control (no Diabetes Dx/Med)</t>
   </si>
   <si>
     <t xml:space="preserve">   78.3 (126) </t>
@@ -695,10 +703,10 @@
     <t xml:space="preserve"> 0.861</t>
   </si>
   <si>
-    <t xml:space="preserve">X.36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diabetes</t>
+    <t>X.36</t>
+  </si>
+  <si>
+    <t>Diabetes</t>
   </si>
   <si>
     <t xml:space="preserve">   21.7 ( 35) </t>
@@ -707,16 +715,16 @@
     <t xml:space="preserve">   22.7 ( 265) </t>
   </si>
   <si>
-    <t xml:space="preserve">Hypertension.selfreport....freq.</t>
+    <t>Hypertension.selfreport....freq.</t>
   </si>
   <si>
     <t xml:space="preserve"> 1.9</t>
   </si>
   <si>
-    <t xml:space="preserve">X.37</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no</t>
+    <t>X.37</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
   <si>
     <t xml:space="preserve">   25.5 ( 41) </t>
@@ -725,10 +733,10 @@
     <t xml:space="preserve">   26.6 ( 310) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.38</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes</t>
+    <t>X.38</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
   <si>
     <t xml:space="preserve">   73.9 (119) </t>
@@ -737,25 +745,25 @@
     <t xml:space="preserve">   71.4 ( 833) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.39</t>
+    <t>X.39</t>
   </si>
   <si>
     <t xml:space="preserve">    2.1 (  24) </t>
   </si>
   <si>
-    <t xml:space="preserve">Hypertension.selfreportdrug....freq.</t>
+    <t>Hypertension.selfreportdrug....freq.</t>
   </si>
   <si>
     <t xml:space="preserve"> 2.4</t>
   </si>
   <si>
-    <t xml:space="preserve">X.40</t>
+    <t>X.40</t>
   </si>
   <si>
     <t xml:space="preserve">   32.9 ( 384) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.41</t>
+    <t>X.41</t>
   </si>
   <si>
     <t xml:space="preserve">   66.5 (107) </t>
@@ -764,22 +772,22 @@
     <t xml:space="preserve">   64.5 ( 753) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.42</t>
+    <t>X.42</t>
   </si>
   <si>
     <t xml:space="preserve">    2.6 (  30) </t>
   </si>
   <si>
-    <t xml:space="preserve">Hypertension.composite....freq.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.43</t>
+    <t>Hypertension.composite....freq.</t>
+  </si>
+  <si>
+    <t>X.43</t>
   </si>
   <si>
     <t xml:space="preserve">   11.2 ( 18) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.44</t>
+    <t>X.44</t>
   </si>
   <si>
     <t xml:space="preserve">   88.8 (143) </t>
@@ -788,13 +796,13 @@
     <t xml:space="preserve">   85.9 (1002) </t>
   </si>
   <si>
-    <t xml:space="preserve">Hypertension.drugs....freq.</t>
+    <t>Hypertension.drugs....freq.</t>
   </si>
   <si>
     <t xml:space="preserve"> 0.2</t>
   </si>
   <si>
-    <t xml:space="preserve">X.45</t>
+    <t>X.45</t>
   </si>
   <si>
     <t xml:space="preserve">   15.5 ( 25) </t>
@@ -803,7 +811,7 @@
     <t xml:space="preserve">   22.8 ( 266) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.46</t>
+    <t>X.46</t>
   </si>
   <si>
     <t xml:space="preserve">   83.9 (135) </t>
@@ -812,16 +820,16 @@
     <t xml:space="preserve">   77.0 ( 899) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.47</t>
+    <t>X.47</t>
   </si>
   <si>
     <t xml:space="preserve">    0.2 (   2) </t>
   </si>
   <si>
-    <t xml:space="preserve">Med.anticoagulants....freq.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.48</t>
+    <t>Med.anticoagulants....freq.</t>
+  </si>
+  <si>
+    <t>X.48</t>
   </si>
   <si>
     <t xml:space="preserve">   89.4 (144) </t>
@@ -830,7 +838,7 @@
     <t xml:space="preserve">   88.0 (1027) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.49</t>
+    <t>X.49</t>
   </si>
   <si>
     <t xml:space="preserve">    9.9 ( 16) </t>
@@ -839,22 +847,22 @@
     <t xml:space="preserve">   11.8 ( 138) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Med.all.antiplatelet....freq.</t>
+    <t>X.50</t>
+  </si>
+  <si>
+    <t>Med.all.antiplatelet....freq.</t>
   </si>
   <si>
     <t xml:space="preserve"> 0.5</t>
   </si>
   <si>
-    <t xml:space="preserve">X.51</t>
+    <t>X.51</t>
   </si>
   <si>
     <t xml:space="preserve">   10.8 ( 126) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.52</t>
+    <t>X.52</t>
   </si>
   <si>
     <t xml:space="preserve">   92.5 (149) </t>
@@ -863,16 +871,16 @@
     <t xml:space="preserve">   88.9 (1037) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.53</t>
+    <t>X.53</t>
   </si>
   <si>
     <t xml:space="preserve">    0.3 (   4) </t>
   </si>
   <si>
-    <t xml:space="preserve">Med.Statin.LLD....freq.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.54</t>
+    <t>Med.Statin.LLD....freq.</t>
+  </si>
+  <si>
+    <t>X.54</t>
   </si>
   <si>
     <t xml:space="preserve">   17.4 ( 28) </t>
@@ -881,7 +889,7 @@
     <t xml:space="preserve">   23.1 ( 270) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.55</t>
+    <t>X.55</t>
   </si>
   <si>
     <t xml:space="preserve">   82.0 (132) </t>
@@ -890,19 +898,19 @@
     <t xml:space="preserve">   76.7 ( 895) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.56</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stroke_Dx....freq.</t>
+    <t>X.56</t>
+  </si>
+  <si>
+    <t>Stroke_Dx....freq.</t>
   </si>
   <si>
     <t xml:space="preserve"> 5.5</t>
   </si>
   <si>
-    <t xml:space="preserve">X.57</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No stroke diagnosed</t>
+    <t>X.57</t>
+  </si>
+  <si>
+    <t>No stroke diagnosed</t>
   </si>
   <si>
     <t xml:space="preserve">   80.1 (129) </t>
@@ -911,232 +919,232 @@
     <t xml:space="preserve">   75.5 ( 881) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.58</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stroke diagnosed</t>
+    <t>X.58</t>
+  </si>
+  <si>
+    <t>Stroke diagnosed</t>
   </si>
   <si>
     <t xml:space="preserve">   19.1 ( 223) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.59</t>
+    <t>X.59</t>
   </si>
   <si>
     <t xml:space="preserve">    5.4 (  63) </t>
   </si>
   <si>
-    <t xml:space="preserve">sympt....freq.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">missing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.60</t>
+    <t>sympt....freq.</t>
+  </si>
+  <si>
+    <t>missing</t>
+  </si>
+  <si>
+    <t>X.60</t>
   </si>
   <si>
     <t xml:space="preserve">  100.0 (161) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.61</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TIA</t>
+    <t>X.61</t>
+  </si>
+  <si>
+    <t>TIA</t>
   </si>
   <si>
     <t xml:space="preserve">   46.5 ( 543) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.62</t>
-  </si>
-  <si>
-    <t xml:space="preserve">minor stroke</t>
+    <t>X.62</t>
+  </si>
+  <si>
+    <t>minor stroke</t>
   </si>
   <si>
     <t xml:space="preserve">   17.1 ( 200) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.63</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Major stroke</t>
+    <t>X.63</t>
+  </si>
+  <si>
+    <t>Major stroke</t>
   </si>
   <si>
     <t xml:space="preserve">   11.7 ( 136) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.64</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amaurosis fugax</t>
+    <t>X.64</t>
+  </si>
+  <si>
+    <t>Amaurosis fugax</t>
   </si>
   <si>
     <t xml:space="preserve">   17.0 ( 198) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.65</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Four vessel disease</t>
+    <t>X.65</t>
+  </si>
+  <si>
+    <t>Four vessel disease</t>
   </si>
   <si>
     <t xml:space="preserve">    2.1 (  25) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.66</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vertebrobasilary TIA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.67</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Retinal infarction</t>
+    <t>X.66</t>
+  </si>
+  <si>
+    <t>Vertebrobasilary TIA</t>
+  </si>
+  <si>
+    <t>X.67</t>
+  </si>
+  <si>
+    <t>Retinal infarction</t>
   </si>
   <si>
     <t xml:space="preserve">    1.4 (  16) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.68</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Symptomatic, but aspecific symtoms</t>
+    <t>X.68</t>
+  </si>
+  <si>
+    <t>Symptomatic, but aspecific symtoms</t>
   </si>
   <si>
     <t xml:space="preserve">    3.1 (  36) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.69</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contralateral symptomatic occlusion</t>
+    <t>X.69</t>
+  </si>
+  <si>
+    <t>Contralateral symptomatic occlusion</t>
   </si>
   <si>
     <t xml:space="preserve">    0.5 (   6) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.70</t>
-  </si>
-  <si>
-    <t xml:space="preserve">retinal infarction</t>
+    <t>X.70</t>
+  </si>
+  <si>
+    <t>retinal infarction</t>
   </si>
   <si>
     <t xml:space="preserve">    0.3 (   3) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.71</t>
-  </si>
-  <si>
-    <t xml:space="preserve">armclaudication due to occlusion subclavian artery, CEA needed for bypass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.72</t>
-  </si>
-  <si>
-    <t xml:space="preserve">retinal infarction + TIAs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.73</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ocular ischemic syndrome</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.74</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ischemisch glaucoom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.75</t>
-  </si>
-  <si>
-    <t xml:space="preserve">subclavian steal syndrome</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.76</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TGA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Symptoms.5G....freq.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.77</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ocular</t>
+    <t>X.71</t>
+  </si>
+  <si>
+    <t>armclaudication due to occlusion subclavian artery, CEA needed for bypass</t>
+  </si>
+  <si>
+    <t>X.72</t>
+  </si>
+  <si>
+    <t>retinal infarction + TIAs</t>
+  </si>
+  <si>
+    <t>X.73</t>
+  </si>
+  <si>
+    <t>Ocular ischemic syndrome</t>
+  </si>
+  <si>
+    <t>X.74</t>
+  </si>
+  <si>
+    <t>ischemisch glaucoom</t>
+  </si>
+  <si>
+    <t>X.75</t>
+  </si>
+  <si>
+    <t>subclavian steal syndrome</t>
+  </si>
+  <si>
+    <t>X.76</t>
+  </si>
+  <si>
+    <t>TGA</t>
+  </si>
+  <si>
+    <t>Symptoms.5G....freq.</t>
+  </si>
+  <si>
+    <t>X.77</t>
+  </si>
+  <si>
+    <t>Ocular</t>
   </si>
   <si>
     <t xml:space="preserve">   17.1 ( 199) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.78</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other</t>
+    <t>X.78</t>
+  </si>
+  <si>
+    <t>Other</t>
   </si>
   <si>
     <t xml:space="preserve">    5.8 (  68) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.79</t>
+    <t>X.79</t>
   </si>
   <si>
     <t xml:space="preserve">    1.6 (  19) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.80</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stroke</t>
+    <t>X.80</t>
+  </si>
+  <si>
+    <t>Stroke</t>
   </si>
   <si>
     <t xml:space="preserve">   28.8 ( 336) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.81</t>
+    <t>X.81</t>
   </si>
   <si>
     <t xml:space="preserve">   46.7 ( 545) </t>
   </si>
   <si>
-    <t xml:space="preserve">AsymptSympt....freq.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.82</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ocular and others</t>
+    <t>AsymptSympt....freq.</t>
+  </si>
+  <si>
+    <t>X.82</t>
+  </si>
+  <si>
+    <t>Ocular and others</t>
   </si>
   <si>
     <t xml:space="preserve">   24.5 ( 286) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.83</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AsymptSympt2G....freq.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.84</t>
+    <t>X.83</t>
+  </si>
+  <si>
+    <t>AsymptSympt2G....freq.</t>
+  </si>
+  <si>
+    <t>X.84</t>
   </si>
   <si>
     <t xml:space="preserve">  100.0 (1167) </t>
   </si>
   <si>
-    <t xml:space="preserve">restenos....freq.</t>
+    <t>restenos....freq.</t>
   </si>
   <si>
     <t xml:space="preserve"> 2.0</t>
   </si>
   <si>
-    <t xml:space="preserve">X.85</t>
-  </si>
-  <si>
-    <t xml:space="preserve">de novo</t>
+    <t>X.85</t>
+  </si>
+  <si>
+    <t>de novo</t>
   </si>
   <si>
     <t xml:space="preserve">   93.2 (150) </t>
@@ -1145,61 +1153,61 @@
     <t xml:space="preserve">   95.0 (1109) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.86</t>
-  </si>
-  <si>
-    <t xml:space="preserve">restenosis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.87</t>
-  </si>
-  <si>
-    <t xml:space="preserve">stenose bij angioseal na PTCA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.88</t>
+    <t>X.86</t>
+  </si>
+  <si>
+    <t>restenosis</t>
+  </si>
+  <si>
+    <t>X.87</t>
+  </si>
+  <si>
+    <t>stenose bij angioseal na PTCA</t>
+  </si>
+  <si>
+    <t>X.88</t>
   </si>
   <si>
     <t xml:space="preserve">    1.9 (  22) </t>
   </si>
   <si>
-    <t xml:space="preserve">stenose....freq.</t>
+    <t>stenose....freq.</t>
   </si>
   <si>
     <t xml:space="preserve"> 2.9</t>
   </si>
   <si>
-    <t xml:space="preserve">X.89</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0-49%</t>
+    <t>X.89</t>
+  </si>
+  <si>
+    <t>0-49%</t>
   </si>
   <si>
     <t xml:space="preserve">    0.6 (   7) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.90</t>
-  </si>
-  <si>
-    <t xml:space="preserve">50-70%</t>
+    <t>X.90</t>
+  </si>
+  <si>
+    <t>50-70%</t>
   </si>
   <si>
     <t xml:space="preserve">    6.3 (  73) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.91</t>
-  </si>
-  <si>
-    <t xml:space="preserve">70-90%</t>
+    <t>X.91</t>
+  </si>
+  <si>
+    <t>70-90%</t>
   </si>
   <si>
     <t xml:space="preserve">   44.6 ( 520) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.92</t>
-  </si>
-  <si>
-    <t xml:space="preserve">90-99%</t>
+    <t>X.92</t>
+  </si>
+  <si>
+    <t>90-99%</t>
   </si>
   <si>
     <t xml:space="preserve">   42.9 ( 69) </t>
@@ -1208,46 +1216,46 @@
     <t xml:space="preserve">   43.3 ( 505) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.93</t>
-  </si>
-  <si>
-    <t xml:space="preserve">100% (Occlusion)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.94</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.95</t>
-  </si>
-  <si>
-    <t xml:space="preserve">50-99%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.96</t>
-  </si>
-  <si>
-    <t xml:space="preserve">70-99%</t>
+    <t>X.93</t>
+  </si>
+  <si>
+    <t>100% (Occlusion)</t>
+  </si>
+  <si>
+    <t>X.94</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>X.95</t>
+  </si>
+  <si>
+    <t>50-99%</t>
+  </si>
+  <si>
+    <t>X.96</t>
+  </si>
+  <si>
+    <t>70-99%</t>
   </si>
   <si>
     <t xml:space="preserve">    1.2 (  14) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.97</t>
-  </si>
-  <si>
-    <t xml:space="preserve">99</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.98</t>
+    <t>X.97</t>
+  </si>
+  <si>
+    <t>99</t>
+  </si>
+  <si>
+    <t>X.98</t>
   </si>
   <si>
     <t xml:space="preserve">    2.8 (  33) </t>
   </si>
   <si>
-    <t xml:space="preserve">MedHx_CVD....freq.</t>
+    <t>MedHx_CVD....freq.</t>
   </si>
   <si>
     <t xml:space="preserve">   37.3 ( 60) </t>
@@ -1259,7 +1267,7 @@
     <t xml:space="preserve"> 0.970</t>
   </si>
   <si>
-    <t xml:space="preserve">X.99</t>
+    <t>X.99</t>
   </si>
   <si>
     <t xml:space="preserve">   62.7 (101) </t>
@@ -1268,13 +1276,13 @@
     <t xml:space="preserve">   63.2 ( 738) </t>
   </si>
   <si>
-    <t xml:space="preserve">CAD_history....freq.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No history CAD</t>
+    <t>CAD_history....freq.</t>
+  </si>
+  <si>
+    <t>X.100</t>
+  </si>
+  <si>
+    <t>No history CAD</t>
   </si>
   <si>
     <t xml:space="preserve">   59.0 ( 95) </t>
@@ -1283,10 +1291,10 @@
     <t xml:space="preserve">   69.2 ( 807) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.101</t>
-  </si>
-  <si>
-    <t xml:space="preserve">History CAD</t>
+    <t>X.101</t>
+  </si>
+  <si>
+    <t>History CAD</t>
   </si>
   <si>
     <t xml:space="preserve">   41.0 ( 66) </t>
@@ -1295,19 +1303,19 @@
     <t xml:space="preserve">   30.8 ( 360) </t>
   </si>
   <si>
-    <t xml:space="preserve">PAOD....freq.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">missing/no data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.102</t>
+    <t>PAOD....freq.</t>
+  </si>
+  <si>
+    <t>missing/no data</t>
+  </si>
+  <si>
+    <t>X.102</t>
   </si>
   <si>
     <t xml:space="preserve">   79.9 ( 932) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.103</t>
+    <t>X.103</t>
   </si>
   <si>
     <t xml:space="preserve">   26.1 ( 42) </t>
@@ -1316,7 +1324,7 @@
     <t xml:space="preserve">   20.1 ( 235) </t>
   </si>
   <si>
-    <t xml:space="preserve">Peripheral.interv....freq.</t>
+    <t>Peripheral.interv....freq.</t>
   </si>
   <si>
     <t xml:space="preserve">   72.7 (117) </t>
@@ -1328,7 +1336,7 @@
     <t xml:space="preserve"> 0.004</t>
   </si>
   <si>
-    <t xml:space="preserve">X.104</t>
+    <t>X.104</t>
   </si>
   <si>
     <t xml:space="preserve">   27.3 ( 44) </t>
@@ -1337,22 +1345,22 @@
     <t xml:space="preserve">   16.7 ( 195) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.105</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EP_composite....freq.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No data available.</t>
+    <t>X.105</t>
+  </si>
+  <si>
+    <t>EP_composite....freq.</t>
+  </si>
+  <si>
+    <t>No data available.</t>
   </si>
   <si>
     <t xml:space="preserve"> 0.8</t>
   </si>
   <si>
-    <t xml:space="preserve">X.106</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No composite endpoints</t>
+    <t>X.106</t>
+  </si>
+  <si>
+    <t>No composite endpoints</t>
   </si>
   <si>
     <t xml:space="preserve">   68.3 (110) </t>
@@ -1361,10 +1369,10 @@
     <t xml:space="preserve">   73.9 ( 862) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.107</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Composite endpoints</t>
+    <t>X.107</t>
+  </si>
+  <si>
+    <t>Composite endpoints</t>
   </si>
   <si>
     <t xml:space="preserve">   31.7 ( 51) </t>
@@ -1373,10 +1381,10 @@
     <t xml:space="preserve">   25.2 ( 294) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.108</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EP_composite_time..mean..SD..</t>
+    <t>X.108</t>
+  </si>
+  <si>
+    <t>EP_composite_time..mean..SD..</t>
   </si>
   <si>
     <t xml:space="preserve">  2.579 (0.961)</t>
@@ -1391,7 +1399,7 @@
     <t xml:space="preserve"> 1.0</t>
   </si>
   <si>
-    <t xml:space="preserve">macmean0..mean..SD..</t>
+    <t>macmean0..mean..SD..</t>
   </si>
   <si>
     <t xml:space="preserve">  0.802 (1.072)</t>
@@ -1406,7 +1414,7 @@
     <t xml:space="preserve"> 2.2</t>
   </si>
   <si>
-    <t xml:space="preserve">smcmean0..mean..SD..</t>
+    <t>smcmean0..mean..SD..</t>
   </si>
   <si>
     <t xml:space="preserve">  2.445 (2.594)</t>
@@ -1421,10 +1429,10 @@
     <t xml:space="preserve"> 2.5</t>
   </si>
   <si>
-    <t xml:space="preserve">Macrophages.bin....freq.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no/minor</t>
+    <t>Macrophages.bin....freq.</t>
+  </si>
+  <si>
+    <t>no/minor</t>
   </si>
   <si>
     <t xml:space="preserve">   50.3 ( 81) </t>
@@ -1439,10 +1447,10 @@
     <t xml:space="preserve"> 1.8</t>
   </si>
   <si>
-    <t xml:space="preserve">X.109</t>
-  </si>
-  <si>
-    <t xml:space="preserve">moderate/heavy</t>
+    <t>X.109</t>
+  </si>
+  <si>
+    <t>moderate/heavy</t>
   </si>
   <si>
     <t xml:space="preserve">   49.1 ( 79) </t>
@@ -1451,13 +1459,13 @@
     <t xml:space="preserve">   52.3 ( 610) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.110</t>
+    <t>X.110</t>
   </si>
   <si>
     <t xml:space="preserve">    2.0 (  23) </t>
   </si>
   <si>
-    <t xml:space="preserve">SMC.bin....freq.</t>
+    <t>SMC.bin....freq.</t>
   </si>
   <si>
     <t xml:space="preserve">   32.5 ( 379) </t>
@@ -1469,46 +1477,46 @@
     <t xml:space="preserve"> 1.7</t>
   </si>
   <si>
-    <t xml:space="preserve">X.111</t>
+    <t>X.111</t>
   </si>
   <si>
     <t xml:space="preserve">   65.8 ( 768) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.112</t>
+    <t>X.112</t>
   </si>
   <si>
     <t xml:space="preserve">    1.7 (  20) </t>
   </si>
   <si>
-    <t xml:space="preserve">neutrophils..mean..SD..</t>
-  </si>
-  <si>
-    <t xml:space="preserve">133.447 (437.032)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">158.140 (448.512)</t>
+    <t>neutrophils..mean..SD..</t>
+  </si>
+  <si>
+    <t>133.447 (437.032)</t>
+  </si>
+  <si>
+    <t>158.140 (448.512)</t>
   </si>
   <si>
     <t xml:space="preserve"> 0.754</t>
   </si>
   <si>
-    <t xml:space="preserve">80.9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mast_cells_plaque..mean..SD..</t>
-  </si>
-  <si>
-    <t xml:space="preserve">123.389 (135.924)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">173.244 (168.601)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">83.7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IPH.bin....freq.</t>
+    <t>80.9</t>
+  </si>
+  <si>
+    <t>Mast_cells_plaque..mean..SD..</t>
+  </si>
+  <si>
+    <t>123.389 (135.924)</t>
+  </si>
+  <si>
+    <t>173.244 (168.601)</t>
+  </si>
+  <si>
+    <t>83.7</t>
+  </si>
+  <si>
+    <t>IPH.bin....freq.</t>
   </si>
   <si>
     <t xml:space="preserve">   39.1 ( 63) </t>
@@ -1523,7 +1531,7 @@
     <t xml:space="preserve"> 1.5</t>
   </si>
   <si>
-    <t xml:space="preserve">X.113</t>
+    <t>X.113</t>
   </si>
   <si>
     <t xml:space="preserve">   60.2 ( 97) </t>
@@ -1532,10 +1540,10 @@
     <t xml:space="preserve">   62.0 ( 723) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.114</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vessel_density_averaged..mean..SD..</t>
+    <t>X.114</t>
+  </si>
+  <si>
+    <t>vessel_density_averaged..mean..SD..</t>
   </si>
   <si>
     <t xml:space="preserve">  8.837 (6.727)</t>
@@ -1550,7 +1558,7 @@
     <t xml:space="preserve"> 8.0</t>
   </si>
   <si>
-    <t xml:space="preserve">Calc.bin....freq.</t>
+    <t>Calc.bin....freq.</t>
   </si>
   <si>
     <t xml:space="preserve">   51.2 ( 597) </t>
@@ -1562,7 +1570,7 @@
     <t xml:space="preserve"> 1.4</t>
   </si>
   <si>
-    <t xml:space="preserve">X.115</t>
+    <t>X.115</t>
   </si>
   <si>
     <t xml:space="preserve">   60.9 ( 98) </t>
@@ -1571,13 +1579,13 @@
     <t xml:space="preserve">   47.3 ( 552) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.116</t>
+    <t>X.116</t>
   </si>
   <si>
     <t xml:space="preserve">    1.5 (  18) </t>
   </si>
   <si>
-    <t xml:space="preserve">Collagen.bin....freq.</t>
+    <t>Collagen.bin....freq.</t>
   </si>
   <si>
     <t xml:space="preserve">   18.6 ( 30) </t>
@@ -1589,7 +1597,7 @@
     <t xml:space="preserve"> 0.528</t>
   </si>
   <si>
-    <t xml:space="preserve">X.117</t>
+    <t>X.117</t>
   </si>
   <si>
     <t xml:space="preserve">   80.7 (130) </t>
@@ -1598,10 +1606,10 @@
     <t xml:space="preserve">   77.8 ( 908) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.118</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fat.bin_10....freq.</t>
+    <t>X.118</t>
+  </si>
+  <si>
+    <t>Fat.bin_10....freq.</t>
   </si>
   <si>
     <t xml:space="preserve"> &lt;10%</t>
@@ -1619,7 +1627,7 @@
     <t xml:space="preserve"> 1.3</t>
   </si>
   <si>
-    <t xml:space="preserve">X.119</t>
+    <t>X.119</t>
   </si>
   <si>
     <t xml:space="preserve"> &gt;10%</t>
@@ -1631,16 +1639,16 @@
     <t xml:space="preserve">   72.8 ( 850) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.120</t>
+    <t>X.120</t>
   </si>
   <si>
     <t xml:space="preserve">    1.5 (  17) </t>
   </si>
   <si>
-    <t xml:space="preserve">Fat.bin_40....freq.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;40%</t>
+    <t>Fat.bin_40....freq.</t>
+  </si>
+  <si>
+    <t>&lt;40%</t>
   </si>
   <si>
     <t xml:space="preserve">   70.5 ( 823) </t>
@@ -1649,22 +1657,22 @@
     <t xml:space="preserve"> 0.061</t>
   </si>
   <si>
-    <t xml:space="preserve">X.121</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&gt;40%</t>
+    <t>X.121</t>
+  </si>
+  <si>
+    <t>&gt;40%</t>
   </si>
   <si>
     <t xml:space="preserve">   28.0 ( 327) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.122</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OverallPlaquePhenotype....freq.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">atheromatous</t>
+    <t>X.122</t>
+  </si>
+  <si>
+    <t>OverallPlaquePhenotype....freq.</t>
+  </si>
+  <si>
+    <t>atheromatous</t>
   </si>
   <si>
     <t xml:space="preserve">   21.1 ( 34) </t>
@@ -1676,19 +1684,19 @@
     <t xml:space="preserve"> 0.019</t>
   </si>
   <si>
-    <t xml:space="preserve">X.123</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fibroatheromatous</t>
+    <t>X.123</t>
+  </si>
+  <si>
+    <t>fibroatheromatous</t>
   </si>
   <si>
     <t xml:space="preserve">   32.9 ( 53) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.124</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fibrous</t>
+    <t>X.124</t>
+  </si>
+  <si>
+    <t>fibrous</t>
   </si>
   <si>
     <t xml:space="preserve">   45.3 ( 73) </t>
@@ -1697,25 +1705,25 @@
     <t xml:space="preserve">   33.5 ( 391) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.125</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IL6..mean..SD..</t>
+    <t>X.125</t>
+  </si>
+  <si>
+    <t>IL6..mean..SD..</t>
   </si>
   <si>
     <t xml:space="preserve"> 85.667 (122.279)</t>
   </si>
   <si>
-    <t xml:space="preserve">103.046 (319.511)</t>
+    <t>103.046 (319.511)</t>
   </si>
   <si>
     <t xml:space="preserve"> 0.616</t>
   </si>
   <si>
-    <t xml:space="preserve">61.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IL6_pg_ug_2015..mean..SD..</t>
+    <t>61.1</t>
+  </si>
+  <si>
+    <t>IL6_pg_ug_2015..mean..SD..</t>
   </si>
   <si>
     <t xml:space="preserve">  0.064 (0.081)</t>
@@ -1727,10 +1735,10 @@
     <t xml:space="preserve"> 0.114</t>
   </si>
   <si>
-    <t xml:space="preserve">13.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IL6R_pg_ug_2015..mean..SD..</t>
+    <t>13.3</t>
+  </si>
+  <si>
+    <t>IL6R_pg_ug_2015..mean..SD..</t>
   </si>
   <si>
     <t xml:space="preserve">  0.233 (0.264)</t>
@@ -1742,25 +1750,25 @@
     <t xml:space="preserve"> 0.306</t>
   </si>
   <si>
-    <t xml:space="preserve">13.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MCP1..mean..SD..</t>
-  </si>
-  <si>
-    <t xml:space="preserve">114.177 (141.121)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">139.853 (115.315)</t>
+    <t>13.1</t>
+  </si>
+  <si>
+    <t>MCP1..mean..SD..</t>
+  </si>
+  <si>
+    <t>114.177 (141.121)</t>
+  </si>
+  <si>
+    <t>139.853 (115.315)</t>
   </si>
   <si>
     <t xml:space="preserve"> 0.063</t>
   </si>
   <si>
-    <t xml:space="preserve">57.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MCP1_pg_ug_2015..mean..SD..</t>
+    <t>57.5</t>
+  </si>
+  <si>
+    <t>MCP1_pg_ug_2015..mean..SD..</t>
   </si>
   <si>
     <t xml:space="preserve">  0.495 (0.818)</t>
@@ -1775,13 +1783,13 @@
     <t xml:space="preserve"> 9.8</t>
   </si>
   <si>
-    <t xml:space="preserve">MCP1_pg_ml_2015..mean..SD..</t>
-  </si>
-  <si>
-    <t xml:space="preserve">405.182 (563.654)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">624.885 (885.359)</t>
+    <t>MCP1_pg_ml_2015..mean..SD..</t>
+  </si>
+  <si>
+    <t>405.182 (563.654)</t>
+  </si>
+  <si>
+    <t>624.885 (885.359)</t>
   </si>
   <si>
     <t xml:space="preserve"> 0.006</t>
@@ -1790,9 +1798,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1828,6 +1835,15 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -2109,14 +2125,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G189"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2139,7 +2165,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -2162,7 +2188,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -2185,7 +2211,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -2208,7 +2234,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -2231,7 +2257,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -2254,7 +2280,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -2277,7 +2303,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>34</v>
       </c>
@@ -2300,7 +2326,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>38</v>
       </c>
@@ -2323,7 +2349,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>42</v>
       </c>
@@ -2346,7 +2372,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>46</v>
       </c>
@@ -2369,7 +2395,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -2392,7 +2418,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>54</v>
       </c>
@@ -2415,7 +2441,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>57</v>
       </c>
@@ -2438,7 +2464,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>61</v>
       </c>
@@ -2461,7 +2487,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>65</v>
       </c>
@@ -2484,7 +2510,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>68</v>
       </c>
@@ -2507,7 +2533,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>71</v>
       </c>
@@ -2530,7 +2556,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>74</v>
       </c>
@@ -2553,7 +2579,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>76</v>
       </c>
@@ -2576,7 +2602,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>78</v>
       </c>
@@ -2599,7 +2625,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>80</v>
       </c>
@@ -2622,7 +2648,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>82</v>
       </c>
@@ -2645,7 +2671,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>84</v>
       </c>
@@ -2668,7 +2694,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>88</v>
       </c>
@@ -2691,7 +2717,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>93</v>
       </c>
@@ -2714,7 +2740,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>97</v>
       </c>
@@ -2737,7 +2763,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>102</v>
       </c>
@@ -2760,7 +2786,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>107</v>
       </c>
@@ -2783,7 +2809,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>112</v>
       </c>
@@ -2806,7 +2832,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>117</v>
       </c>
@@ -2829,7 +2855,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>120</v>
       </c>
@@ -2852,7 +2878,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>123</v>
       </c>
@@ -2875,7 +2901,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>126</v>
       </c>
@@ -2898,7 +2924,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>129</v>
       </c>
@@ -2921,7 +2947,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>134</v>
       </c>
@@ -2944,7 +2970,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>139</v>
       </c>
@@ -2967,7 +2993,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>143</v>
       </c>
@@ -2990,7 +3016,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>148</v>
       </c>
@@ -3013,7 +3039,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>153</v>
       </c>
@@ -3036,7 +3062,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>154</v>
       </c>
@@ -3059,7 +3085,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>158</v>
       </c>
@@ -3082,7 +3108,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>162</v>
       </c>
@@ -3105,7 +3131,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>166</v>
       </c>
@@ -3128,7 +3154,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>169</v>
       </c>
@@ -3151,11 +3177,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>173</v>
       </c>
-      <c r="B46"/>
       <c r="C46" t="s">
         <v>174</v>
       </c>
@@ -3172,7 +3197,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>176</v>
       </c>
@@ -3195,7 +3220,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>178</v>
       </c>
@@ -3218,7 +3243,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>182</v>
       </c>
@@ -3241,7 +3266,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>186</v>
       </c>
@@ -3264,7 +3289,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>190</v>
       </c>
@@ -3287,11 +3312,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>193</v>
       </c>
-      <c r="B52"/>
       <c r="C52" t="s">
         <v>194</v>
       </c>
@@ -3308,7 +3332,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>195</v>
       </c>
@@ -3331,7 +3355,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>201</v>
       </c>
@@ -3354,7 +3378,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>204</v>
       </c>
@@ -3377,11 +3401,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>207</v>
       </c>
-      <c r="B56"/>
       <c r="C56" t="s">
         <v>208</v>
       </c>
@@ -3398,7 +3421,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>210</v>
       </c>
@@ -3421,7 +3444,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>216</v>
       </c>
@@ -3444,11 +3467,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>220</v>
       </c>
-      <c r="B59"/>
       <c r="C59" t="s">
         <v>221</v>
       </c>
@@ -3465,7 +3487,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>222</v>
       </c>
@@ -3488,7 +3510,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>227</v>
       </c>
@@ -3511,7 +3533,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>231</v>
       </c>
@@ -3534,7 +3556,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>233</v>
       </c>
@@ -3557,7 +3579,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>237</v>
       </c>
@@ -3580,11 +3602,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>241</v>
       </c>
-      <c r="B65"/>
       <c r="C65" t="s">
         <v>171</v>
       </c>
@@ -3601,7 +3622,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>243</v>
       </c>
@@ -3624,7 +3645,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="67">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>245</v>
       </c>
@@ -3647,7 +3668,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="68">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>247</v>
       </c>
@@ -3670,11 +3691,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>250</v>
       </c>
-      <c r="B69"/>
       <c r="C69" t="s">
         <v>180</v>
       </c>
@@ -3691,7 +3711,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="70">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>252</v>
       </c>
@@ -3714,7 +3734,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="71">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>253</v>
       </c>
@@ -3737,7 +3757,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="72">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>255</v>
       </c>
@@ -3760,7 +3780,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>258</v>
       </c>
@@ -3783,7 +3803,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="74">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>260</v>
       </c>
@@ -3806,7 +3826,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="75">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>263</v>
       </c>
@@ -3829,11 +3849,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="76">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>266</v>
       </c>
-      <c r="B76"/>
       <c r="C76" t="s">
         <v>171</v>
       </c>
@@ -3850,7 +3869,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="77">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>268</v>
       </c>
@@ -3873,7 +3892,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="78">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>269</v>
       </c>
@@ -3896,7 +3915,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="79">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>272</v>
       </c>
@@ -3919,11 +3938,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="80">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>275</v>
       </c>
-      <c r="B80"/>
       <c r="C80" t="s">
         <v>171</v>
       </c>
@@ -3940,7 +3958,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="81">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>276</v>
       </c>
@@ -3963,7 +3981,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="82">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>278</v>
       </c>
@@ -3986,7 +4004,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="83">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>280</v>
       </c>
@@ -4009,11 +4027,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="84">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>283</v>
       </c>
-      <c r="B84"/>
       <c r="C84" t="s">
         <v>180</v>
       </c>
@@ -4030,7 +4047,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="85">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>285</v>
       </c>
@@ -4053,7 +4070,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="86">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>286</v>
       </c>
@@ -4076,7 +4093,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="87">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>289</v>
       </c>
@@ -4099,11 +4116,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="88">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>292</v>
       </c>
-      <c r="B88"/>
       <c r="C88" t="s">
         <v>171</v>
       </c>
@@ -4120,7 +4136,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="89">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>293</v>
       </c>
@@ -4143,7 +4159,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="90">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>295</v>
       </c>
@@ -4166,7 +4182,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="91">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>299</v>
       </c>
@@ -4189,11 +4205,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="92">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>302</v>
       </c>
-      <c r="B92"/>
       <c r="C92" t="s">
         <v>52</v>
       </c>
@@ -4210,7 +4225,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="93">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>304</v>
       </c>
@@ -4233,7 +4248,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="94">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>306</v>
       </c>
@@ -4256,7 +4271,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="95">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>308</v>
       </c>
@@ -4279,7 +4294,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="96">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>311</v>
       </c>
@@ -4302,7 +4317,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="97">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>314</v>
       </c>
@@ -4325,7 +4340,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="98">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>317</v>
       </c>
@@ -4348,7 +4363,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="99">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>320</v>
       </c>
@@ -4371,7 +4386,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="100">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>323</v>
       </c>
@@ -4394,7 +4409,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="101">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>325</v>
       </c>
@@ -4417,7 +4432,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="102">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>328</v>
       </c>
@@ -4440,7 +4455,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="103">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>331</v>
       </c>
@@ -4463,7 +4478,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="104">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>334</v>
       </c>
@@ -4486,7 +4501,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="105">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>337</v>
       </c>
@@ -4509,7 +4524,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="106">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>339</v>
       </c>
@@ -4532,7 +4547,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="107">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>341</v>
       </c>
@@ -4555,7 +4570,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="108">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>343</v>
       </c>
@@ -4578,7 +4593,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="109">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>345</v>
       </c>
@@ -4601,7 +4616,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="110">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>347</v>
       </c>
@@ -4624,7 +4639,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="111">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>349</v>
       </c>
@@ -4647,7 +4662,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="112">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>350</v>
       </c>
@@ -4670,7 +4685,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="113">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>353</v>
       </c>
@@ -4693,7 +4708,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="114">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>356</v>
       </c>
@@ -4716,7 +4731,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="115">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>358</v>
       </c>
@@ -4739,7 +4754,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="116">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>361</v>
       </c>
@@ -4762,7 +4777,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="117">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>363</v>
       </c>
@@ -4785,7 +4800,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="118">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>364</v>
       </c>
@@ -4808,7 +4823,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="119">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>367</v>
       </c>
@@ -4831,7 +4846,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="120">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>368</v>
       </c>
@@ -4854,7 +4869,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="121">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>369</v>
       </c>
@@ -4877,7 +4892,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="122">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>371</v>
       </c>
@@ -4900,7 +4915,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="123">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>373</v>
       </c>
@@ -4923,7 +4938,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="124">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>377</v>
       </c>
@@ -4946,7 +4961,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="125">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>379</v>
       </c>
@@ -4969,11 +4984,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="126">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>381</v>
       </c>
-      <c r="B126"/>
       <c r="C126" t="s">
         <v>194</v>
       </c>
@@ -4990,7 +5004,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="127">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>383</v>
       </c>
@@ -5013,7 +5027,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="128">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>385</v>
       </c>
@@ -5036,7 +5050,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="129">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>388</v>
       </c>
@@ -5059,7 +5073,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="130">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>391</v>
       </c>
@@ -5082,7 +5096,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="131">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>394</v>
       </c>
@@ -5105,7 +5119,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="132">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>398</v>
       </c>
@@ -5128,7 +5142,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="133">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>400</v>
       </c>
@@ -5151,7 +5165,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="134">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>402</v>
       </c>
@@ -5174,7 +5188,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="135">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>404</v>
       </c>
@@ -5197,7 +5211,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="136">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>407</v>
       </c>
@@ -5220,11 +5234,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="137">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>409</v>
       </c>
-      <c r="B137"/>
       <c r="C137" t="s">
         <v>194</v>
       </c>
@@ -5241,7 +5254,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="138">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>411</v>
       </c>
@@ -5264,7 +5277,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="139">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>415</v>
       </c>
@@ -5287,7 +5300,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="140">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>418</v>
       </c>
@@ -5310,7 +5323,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="141">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>419</v>
       </c>
@@ -5333,7 +5346,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="142">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>423</v>
       </c>
@@ -5356,7 +5369,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="143">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>427</v>
       </c>
@@ -5379,7 +5392,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="144">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>429</v>
       </c>
@@ -5402,7 +5415,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="145">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>431</v>
       </c>
@@ -5425,7 +5438,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="146">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>434</v>
       </c>
@@ -5448,7 +5461,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="147">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>438</v>
       </c>
@@ -5471,11 +5484,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="148">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>441</v>
       </c>
-      <c r="B148"/>
       <c r="C148" t="s">
         <v>23</v>
       </c>
@@ -5492,7 +5504,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="149">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>442</v>
       </c>
@@ -5515,7 +5527,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="150">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>445</v>
       </c>
@@ -5538,7 +5550,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="151">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>449</v>
       </c>
@@ -5561,11 +5573,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="152">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>453</v>
       </c>
-      <c r="B152"/>
       <c r="C152" t="s">
         <v>23</v>
       </c>
@@ -5582,7 +5593,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="153">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>454</v>
       </c>
@@ -5605,7 +5616,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="154">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>459</v>
       </c>
@@ -5628,7 +5639,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="155">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>464</v>
       </c>
@@ -5651,7 +5662,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="156">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>469</v>
       </c>
@@ -5674,7 +5685,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="157">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>475</v>
       </c>
@@ -5697,11 +5708,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="158">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>479</v>
       </c>
-      <c r="B158"/>
       <c r="C158" t="s">
         <v>171</v>
       </c>
@@ -5718,7 +5728,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="159">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>481</v>
       </c>
@@ -5741,7 +5751,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="160">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>485</v>
       </c>
@@ -5764,11 +5774,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="161">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>487</v>
       </c>
-      <c r="B161"/>
       <c r="C161" t="s">
         <v>180</v>
       </c>
@@ -5785,7 +5794,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="162">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>489</v>
       </c>
@@ -5808,7 +5817,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="163">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>494</v>
       </c>
@@ -5831,7 +5840,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="164">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>498</v>
       </c>
@@ -5854,7 +5863,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="165">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>503</v>
       </c>
@@ -5877,11 +5886,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="166">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>506</v>
       </c>
-      <c r="B166"/>
       <c r="C166" t="s">
         <v>171</v>
       </c>
@@ -5898,7 +5906,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="167">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>507</v>
       </c>
@@ -5921,7 +5929,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="168">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>512</v>
       </c>
@@ -5944,7 +5952,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="169">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>516</v>
       </c>
@@ -5967,11 +5975,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="170">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>519</v>
       </c>
-      <c r="B170"/>
       <c r="C170" t="s">
         <v>23</v>
       </c>
@@ -5988,7 +5995,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="171">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>521</v>
       </c>
@@ -6011,7 +6018,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="172">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>525</v>
       </c>
@@ -6034,11 +6041,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="173">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>528</v>
       </c>
-      <c r="B173"/>
       <c r="C173" t="s">
         <v>171</v>
       </c>
@@ -6055,7 +6061,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="174">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>529</v>
       </c>
@@ -6078,7 +6084,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="175">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>535</v>
       </c>
@@ -6101,11 +6107,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="176">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>539</v>
       </c>
-      <c r="B176"/>
       <c r="C176" t="s">
         <v>23</v>
       </c>
@@ -6122,7 +6127,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="177">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>541</v>
       </c>
@@ -6145,7 +6150,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="178">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>545</v>
       </c>
@@ -6168,11 +6173,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="179">
+    <row r="179" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>548</v>
       </c>
-      <c r="B179"/>
       <c r="C179" t="s">
         <v>23</v>
       </c>
@@ -6189,7 +6193,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="180">
+    <row r="180" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>549</v>
       </c>
@@ -6212,7 +6216,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="181">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>554</v>
       </c>
@@ -6235,7 +6239,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="182">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>557</v>
       </c>
@@ -6258,11 +6262,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="183">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>561</v>
       </c>
-      <c r="B183"/>
       <c r="C183" t="s">
         <v>171</v>
       </c>
@@ -6279,7 +6282,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="184">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>562</v>
       </c>
@@ -6302,7 +6305,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="185">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>567</v>
       </c>
@@ -6325,7 +6328,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="186">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>572</v>
       </c>
@@ -6348,7 +6351,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="187">
+    <row r="187" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>577</v>
       </c>
@@ -6371,7 +6374,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="188">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>582</v>
       </c>
@@ -6394,7 +6397,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="189">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>587</v>
       </c>
@@ -6419,6 +6422,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>